<commit_message>
got rid of washington sample
</commit_message>
<xml_diff>
--- a/data/01_pd-samples/26_01_15_pd_samples-edited.xlsx
+++ b/data/01_pd-samples/26_01_15_pd_samples-edited.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caprinapugliese/Documents/School/Uconn/2024-26_Grad_School/Dagilis-lab/WNS-project/data/01_pd-samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A276634A-4471-0645-BCB5-C744ECC66C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4118014C-9462-8646-B4A1-605D4A34AC68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27740" windowHeight="17500" xr2:uid="{D99E271A-162C-F24C-8D0E-BBA6ED327C07}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27740" windowHeight="17500" activeTab="3" xr2:uid="{D99E271A-162C-F24C-8D0E-BBA6ED327C07}"/>
   </bookViews>
   <sheets>
     <sheet name="25_10-16_pd_samples-edited" sheetId="1" r:id="rId1"/>
     <sheet name="pd_northamer_only" sheetId="2" r:id="rId2"/>
     <sheet name="NoA_Pd_coords" sheetId="3" r:id="rId3"/>
+    <sheet name="no washington" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1787" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="422">
   <si>
     <t>sample_id</t>
   </si>
@@ -1956,7 +1957,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2CB732F1-CFFD-B246-B3FF-1A39A44F848B}" name="Table13" displayName="Table13" ref="A1:X52" totalsRowShown="0">
   <autoFilter ref="A1:X52" xr:uid="{90C14361-2949-B74A-BFF6-1CEFD0790204}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X52">
-    <sortCondition descending="1" ref="R1:R52"/>
+    <sortCondition ref="B1:B52"/>
   </sortState>
   <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{684E08F5-2427-9C44-9268-566A0648100F}" name="sample_id"/>
@@ -2307,7 +2308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E4D9535-1238-AB48-B467-419735026371}">
   <dimension ref="A1:X75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -6768,8 +6769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BD2066C-9D82-5444-90C3-5EB5DCC8324A}">
   <dimension ref="A1:X52"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R53" sqref="R53"/>
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6869,92 +6870,98 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
       <c r="D2" s="5">
-        <v>5755622</v>
+        <v>3545531</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="H2">
-        <v>2013</v>
+        <v>2016</v>
       </c>
       <c r="I2">
-        <v>2013</v>
+        <v>2016</v>
       </c>
       <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" t="s">
+        <v>298</v>
+      </c>
+      <c r="N2" t="s">
+        <v>302</v>
+      </c>
+      <c r="O2" t="s">
+        <v>309</v>
+      </c>
+      <c r="P2" t="s">
+        <v>406</v>
+      </c>
+      <c r="Q2" s="8">
+        <v>43.0274</v>
+      </c>
+      <c r="R2" s="8">
+        <v>-90.092200000000005</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="X2" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="5">
+        <v>5755618</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3">
+        <v>2015</v>
+      </c>
+      <c r="I3">
+        <v>2015</v>
+      </c>
+      <c r="J3" t="s">
         <v>42</v>
-      </c>
-      <c r="K2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" t="s">
-        <v>291</v>
-      </c>
-      <c r="N2" t="s">
-        <v>295</v>
-      </c>
-      <c r="O2" t="s">
-        <v>305</v>
-      </c>
-      <c r="Q2">
-        <v>46.011941999999998</v>
-      </c>
-      <c r="R2">
-        <v>-62.618592999999997</v>
-      </c>
-      <c r="U2" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D3" s="5">
-        <v>7191698</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="F3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" t="s">
-        <v>121</v>
-      </c>
-      <c r="H3">
-        <v>2012</v>
-      </c>
-      <c r="I3" s="1">
-        <v>41013</v>
-      </c>
-      <c r="J3" t="s">
-        <v>117</v>
       </c>
       <c r="K3" t="s">
         <v>43</v>
@@ -6966,45 +6973,63 @@
         <v>291</v>
       </c>
       <c r="N3" t="s">
-        <v>295</v>
+        <v>319</v>
       </c>
       <c r="O3" t="s">
-        <v>296</v>
+        <v>320</v>
+      </c>
+      <c r="P3" t="s">
+        <v>406</v>
       </c>
       <c r="Q3">
-        <v>46.011941999999998</v>
+        <v>48.498627856338103</v>
       </c>
       <c r="R3">
-        <v>-62.618592999999997</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+        <v>-89.227383734950806</v>
+      </c>
+      <c r="S3" t="s">
+        <v>415</v>
+      </c>
+      <c r="T3" t="s">
+        <v>414</v>
+      </c>
+      <c r="U3" t="s">
+        <v>321</v>
+      </c>
+      <c r="V3" t="s">
+        <v>412</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D4" s="5">
-        <v>5755620</v>
+        <v>5755619</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F4" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H4">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="I4">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="J4" t="s">
         <v>42</v>
@@ -7019,45 +7044,57 @@
         <v>291</v>
       </c>
       <c r="N4" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="O4" t="s">
-        <v>305</v>
+        <v>320</v>
+      </c>
+      <c r="P4" t="s">
+        <v>406</v>
       </c>
       <c r="Q4">
-        <v>45.003125911591702</v>
+        <v>48.498627856338103</v>
       </c>
       <c r="R4">
-        <v>-63.830206168139703</v>
+        <v>-89.227383734950806</v>
+      </c>
+      <c r="S4" t="s">
+        <v>415</v>
+      </c>
+      <c r="T4" t="s">
+        <v>414</v>
       </c>
       <c r="U4" t="s">
-        <v>307</v>
+        <v>321</v>
+      </c>
+      <c r="V4" t="s">
+        <v>413</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D5" s="5">
-        <v>5755621</v>
+        <v>5755620</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F5" t="s">
         <v>51</v>
       </c>
       <c r="G5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H5">
         <v>2013</v>
@@ -7092,28 +7129,31 @@
       <c r="U5" t="s">
         <v>307</v>
       </c>
+      <c r="W5" s="2" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>277</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>278</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>277</v>
+        <v>53</v>
       </c>
       <c r="D6" s="5">
-        <v>11812089</v>
+        <v>5755621</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>279</v>
+        <v>55</v>
       </c>
       <c r="F6" t="s">
         <v>51</v>
       </c>
       <c r="G6" t="s">
-        <v>280</v>
+        <v>56</v>
       </c>
       <c r="H6">
         <v>2013</v>
@@ -7122,7 +7162,7 @@
         <v>2013</v>
       </c>
       <c r="J6" t="s">
-        <v>117</v>
+        <v>42</v>
       </c>
       <c r="K6" t="s">
         <v>43</v>
@@ -7137,36 +7177,39 @@
         <v>322</v>
       </c>
       <c r="O6" t="s">
-        <v>333</v>
+        <v>305</v>
       </c>
       <c r="Q6">
-        <v>44.992969000000002</v>
+        <v>45.003125911591702</v>
       </c>
       <c r="R6">
-        <v>-64.167955000000006</v>
+        <v>-63.830206168139703</v>
+      </c>
+      <c r="U6" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="D7" s="5">
-        <v>5755630</v>
+        <v>5755622</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
       <c r="F7" t="s">
         <v>51</v>
       </c>
       <c r="G7" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="H7">
         <v>2013</v>
@@ -7187,16 +7230,16 @@
         <v>291</v>
       </c>
       <c r="N7" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="O7" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="Q7">
-        <v>45.93694</v>
+        <v>46.011941999999998</v>
       </c>
       <c r="R7">
-        <v>-64.476939999999999</v>
+        <v>-62.618592999999997</v>
       </c>
       <c r="U7" t="s">
         <v>307</v>
@@ -7204,34 +7247,34 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>114</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>113</v>
+        <v>61</v>
       </c>
       <c r="D8" s="5">
-        <v>7191697</v>
+        <v>5755623</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>115</v>
+        <v>63</v>
       </c>
       <c r="F8" t="s">
         <v>51</v>
       </c>
       <c r="G8" t="s">
-        <v>116</v>
+        <v>64</v>
       </c>
       <c r="H8">
-        <v>2012</v>
-      </c>
-      <c r="I8" s="1">
-        <v>41011</v>
+        <v>2015</v>
+      </c>
+      <c r="I8">
+        <v>2015</v>
       </c>
       <c r="J8" t="s">
-        <v>117</v>
+        <v>42</v>
       </c>
       <c r="K8" t="s">
         <v>43</v>
@@ -7243,48 +7286,51 @@
         <v>291</v>
       </c>
       <c r="N8" t="s">
-        <v>292</v>
+        <v>319</v>
       </c>
       <c r="O8" t="s">
-        <v>297</v>
+        <v>320</v>
       </c>
       <c r="Q8">
-        <v>45.93694</v>
+        <v>48.498627856338103</v>
       </c>
       <c r="R8">
-        <v>-64.476939999999999</v>
+        <v>-89.227383734950806</v>
+      </c>
+      <c r="U8" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>157</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
-        <v>241</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>157</v>
+        <v>65</v>
       </c>
       <c r="D9" s="5">
-        <v>6011488</v>
+        <v>5755624</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>242</v>
+        <v>67</v>
       </c>
       <c r="F9" t="s">
-        <v>232</v>
+        <v>51</v>
       </c>
       <c r="G9" t="s">
-        <v>243</v>
+        <v>68</v>
       </c>
       <c r="H9">
-        <v>2012</v>
-      </c>
-      <c r="I9" s="1">
-        <v>41011</v>
+        <v>2015</v>
+      </c>
+      <c r="I9">
+        <v>2015</v>
       </c>
       <c r="J9" t="s">
-        <v>130</v>
+        <v>42</v>
       </c>
       <c r="K9" t="s">
         <v>43</v>
@@ -7299,36 +7345,39 @@
         <v>292</v>
       </c>
       <c r="O9" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="Q9">
-        <v>45.93694</v>
+        <v>45.913153999999999</v>
       </c>
       <c r="R9">
-        <v>-64.476939999999999</v>
+        <v>-64.671137999999999</v>
+      </c>
+      <c r="U9" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>285</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>286</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>285</v>
+        <v>69</v>
       </c>
       <c r="D10" s="5">
-        <v>11812091</v>
+        <v>5755625</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>287</v>
+        <v>71</v>
       </c>
       <c r="F10" t="s">
         <v>51</v>
       </c>
       <c r="G10" t="s">
-        <v>288</v>
+        <v>72</v>
       </c>
       <c r="H10">
         <v>2012</v>
@@ -7337,7 +7386,7 @@
         <v>2012</v>
       </c>
       <c r="J10" t="s">
-        <v>117</v>
+        <v>42</v>
       </c>
       <c r="K10" t="s">
         <v>43</v>
@@ -7352,42 +7401,45 @@
         <v>292</v>
       </c>
       <c r="O10" t="s">
-        <v>297</v>
+        <v>308</v>
       </c>
       <c r="Q10">
-        <v>45.93694</v>
+        <v>45.8172</v>
       </c>
       <c r="R10">
-        <v>-64.476939999999999</v>
+        <v>-65.610500000000002</v>
+      </c>
+      <c r="U10" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D11" s="5">
-        <v>5755624</v>
+        <v>5755626</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="F11" t="s">
         <v>51</v>
       </c>
       <c r="G11" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="H11">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="I11">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="J11" t="s">
         <v>42</v>
@@ -7405,13 +7457,13 @@
         <v>292</v>
       </c>
       <c r="O11" t="s">
-        <v>293</v>
+        <v>308</v>
       </c>
       <c r="Q11">
-        <v>45.913153999999999</v>
+        <v>45.8172</v>
       </c>
       <c r="R11">
-        <v>-64.671137999999999</v>
+        <v>-65.610500000000002</v>
       </c>
       <c r="U11" t="s">
         <v>307</v>
@@ -7475,25 +7527,25 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="B13" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="C13" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="D13" s="5">
-        <v>5757331</v>
+        <v>5755628</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="F13" t="s">
         <v>51</v>
       </c>
       <c r="G13" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="H13">
         <v>2012</v>
@@ -7517,13 +7569,13 @@
         <v>292</v>
       </c>
       <c r="O13" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="Q13">
-        <v>45.913153999999999</v>
+        <v>45.615960000000001</v>
       </c>
       <c r="R13">
-        <v>-64.671137999999999</v>
+        <v>-65.439909999999998</v>
       </c>
       <c r="U13" t="s">
         <v>307</v>
@@ -7531,31 +7583,31 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B14" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="D14" s="5">
-        <v>5755628</v>
+        <v>5755630</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="F14" t="s">
         <v>51</v>
       </c>
       <c r="G14" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="H14">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="I14">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="J14" t="s">
         <v>42</v>
@@ -7573,13 +7625,13 @@
         <v>292</v>
       </c>
       <c r="O14" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="Q14">
-        <v>45.615960000000001</v>
+        <v>45.93694</v>
       </c>
       <c r="R14">
-        <v>-65.439909999999998</v>
+        <v>-64.476939999999999</v>
       </c>
       <c r="U14" t="s">
         <v>307</v>
@@ -7699,31 +7751,31 @@
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>101</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>101</v>
       </c>
       <c r="D17" s="5">
-        <v>5755625</v>
+        <v>5755633</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="F17" t="s">
         <v>51</v>
       </c>
       <c r="G17" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="H17">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="I17">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="J17" t="s">
         <v>42</v>
@@ -7755,31 +7807,31 @@
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>105</v>
       </c>
       <c r="B18" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
+        <v>105</v>
       </c>
       <c r="D18" s="5">
-        <v>5755626</v>
+        <v>5755634</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="F18" t="s">
         <v>51</v>
       </c>
       <c r="G18" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="H18">
-        <v>2013</v>
+        <v>2008</v>
       </c>
       <c r="I18">
-        <v>2013</v>
+        <v>2008</v>
       </c>
       <c r="J18" t="s">
         <v>42</v>
@@ -7791,51 +7843,60 @@
         <v>20</v>
       </c>
       <c r="M18" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="N18" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="O18" t="s">
-        <v>308</v>
+        <v>300</v>
+      </c>
+      <c r="P18" t="s">
+        <v>406</v>
       </c>
       <c r="Q18">
-        <v>45.8172</v>
+        <v>41.844515371877698</v>
       </c>
       <c r="R18">
-        <v>-65.610500000000002</v>
+        <v>-74.098548155198898</v>
+      </c>
+      <c r="S18" t="s">
+        <v>415</v>
       </c>
       <c r="U18" t="s">
-        <v>307</v>
+        <v>325</v>
+      </c>
+      <c r="V18" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B19" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="C19" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="D19" s="5">
-        <v>5755633</v>
+        <v>5757331</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="F19" t="s">
         <v>51</v>
       </c>
       <c r="G19" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="H19">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="I19">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="J19" t="s">
         <v>42</v>
@@ -7853,13 +7914,13 @@
         <v>292</v>
       </c>
       <c r="O19" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="Q19">
-        <v>45.8172</v>
+        <v>45.913153999999999</v>
       </c>
       <c r="R19">
-        <v>-65.610500000000002</v>
+        <v>-64.671137999999999</v>
       </c>
       <c r="U19" t="s">
         <v>307</v>
@@ -7867,31 +7928,31 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>281</v>
+        <v>113</v>
       </c>
       <c r="B20" t="s">
-        <v>282</v>
+        <v>114</v>
       </c>
       <c r="C20" t="s">
-        <v>281</v>
+        <v>113</v>
       </c>
       <c r="D20" s="5">
-        <v>11812090</v>
+        <v>7191697</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>283</v>
+        <v>115</v>
       </c>
       <c r="F20" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="G20" t="s">
-        <v>284</v>
+        <v>116</v>
       </c>
       <c r="H20">
         <v>2012</v>
       </c>
       <c r="I20" s="1">
-        <v>40967</v>
+        <v>41011</v>
       </c>
       <c r="J20" t="s">
         <v>117</v>
@@ -7909,42 +7970,42 @@
         <v>292</v>
       </c>
       <c r="O20" t="s">
-        <v>332</v>
+        <v>297</v>
       </c>
       <c r="Q20">
-        <v>45.300289999999997</v>
+        <v>45.93694</v>
       </c>
       <c r="R20">
-        <v>-66.050550000000001</v>
+        <v>-64.476939999999999</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>215</v>
+        <v>118</v>
       </c>
       <c r="B21" t="s">
-        <v>261</v>
+        <v>119</v>
       </c>
       <c r="C21" t="s">
-        <v>215</v>
+        <v>118</v>
       </c>
       <c r="D21" s="5">
-        <v>6011495</v>
+        <v>7191698</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>262</v>
+        <v>120</v>
       </c>
       <c r="F21" t="s">
         <v>51</v>
       </c>
       <c r="G21" t="s">
-        <v>263</v>
+        <v>121</v>
       </c>
       <c r="H21">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="I21" s="1">
-        <v>40889</v>
+        <v>41013</v>
       </c>
       <c r="J21" t="s">
         <v>117</v>
@@ -7956,54 +8017,51 @@
         <v>20</v>
       </c>
       <c r="M21" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="N21" t="s">
-        <v>357</v>
+        <v>295</v>
       </c>
       <c r="O21" t="s">
-        <v>372</v>
+        <v>296</v>
       </c>
       <c r="Q21">
-        <v>44.349651999999999</v>
+        <v>46.011941999999998</v>
       </c>
       <c r="R21">
-        <v>-68.211070000000007</v>
-      </c>
-      <c r="X21" s="9" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+        <v>-62.618592999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="B22" t="s">
-        <v>224</v>
+        <v>123</v>
       </c>
       <c r="C22" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="D22" s="5">
-        <v>6011482</v>
+        <v>1952982</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>225</v>
+        <v>124</v>
       </c>
       <c r="F22" t="s">
         <v>51</v>
       </c>
       <c r="G22" t="s">
-        <v>226</v>
+        <v>125</v>
       </c>
       <c r="H22">
-        <v>2010</v>
-      </c>
-      <c r="I22" s="1">
-        <v>40205</v>
+        <v>2008</v>
+      </c>
+      <c r="I22">
+        <v>2008</v>
       </c>
       <c r="J22" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="K22" t="s">
         <v>43</v>
@@ -8015,45 +8073,63 @@
         <v>298</v>
       </c>
       <c r="N22" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="O22" t="s">
-        <v>364</v>
+        <v>328</v>
       </c>
       <c r="Q22">
-        <v>43.451169999999998</v>
+        <v>41.844515371877698</v>
       </c>
       <c r="R22">
-        <v>-72.942554999999999</v>
+        <v>-74.098548155198898</v>
+      </c>
+      <c r="S22" t="s">
+        <v>379</v>
+      </c>
+      <c r="T22" t="s">
+        <v>380</v>
+      </c>
+      <c r="U22" t="s">
+        <v>378</v>
+      </c>
+      <c r="V22" t="s">
+        <v>384</v>
+      </c>
+      <c r="W22" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="X22" s="2" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="B23" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
       <c r="C23" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="D23" s="5">
-        <v>6011475</v>
+        <v>6011469</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
       <c r="F23" t="s">
         <v>51</v>
       </c>
       <c r="G23" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="H23">
         <v>2009</v>
       </c>
       <c r="I23" s="1">
-        <v>39840</v>
+        <v>39897</v>
       </c>
       <c r="J23" t="s">
         <v>130</v>
@@ -8068,45 +8144,45 @@
         <v>298</v>
       </c>
       <c r="N23" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="O23" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="Q23">
-        <v>41.745700999999997</v>
+        <v>40.888610999999997</v>
       </c>
       <c r="R23">
-        <v>-73.158473999999998</v>
+        <v>-77.386111</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>202</v>
+        <v>177</v>
       </c>
       <c r="B24" t="s">
-        <v>213</v>
+        <v>178</v>
       </c>
       <c r="C24" t="s">
-        <v>202</v>
+        <v>177</v>
       </c>
       <c r="D24" s="5">
-        <v>6011478</v>
+        <v>6011470</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>214</v>
+        <v>179</v>
       </c>
       <c r="F24" t="s">
         <v>51</v>
       </c>
       <c r="G24" t="s">
-        <v>215</v>
+        <v>180</v>
       </c>
       <c r="H24">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="I24" s="1">
-        <v>39539</v>
+        <v>39990</v>
       </c>
       <c r="J24" t="s">
         <v>130</v>
@@ -8121,45 +8197,45 @@
         <v>298</v>
       </c>
       <c r="N24" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="O24" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="Q24">
-        <v>41.745700999999997</v>
+        <v>40.877385651285401</v>
       </c>
       <c r="R24">
-        <v>-73.158473999999998</v>
+        <v>-74.968855407371393</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="B25" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="C25" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="D25" s="5">
-        <v>6011477</v>
+        <v>6011471</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
       <c r="F25" t="s">
         <v>51</v>
       </c>
       <c r="G25" t="s">
-        <v>202</v>
+        <v>183</v>
       </c>
       <c r="H25">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="I25" s="1">
-        <v>39528</v>
+        <v>39843</v>
       </c>
       <c r="J25" t="s">
         <v>130</v>
@@ -8174,48 +8250,48 @@
         <v>298</v>
       </c>
       <c r="N25" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="O25" t="s">
-        <v>361</v>
+        <v>344</v>
       </c>
       <c r="Q25">
-        <v>42.592351000000001</v>
+        <v>38.664935999999997</v>
       </c>
       <c r="R25">
-        <v>-73.226241999999999</v>
+        <v>-79.430160999999998</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B26" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C26" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="D26" s="5">
-        <v>6011474</v>
+        <v>6011472</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="F26" t="s">
         <v>51</v>
       </c>
       <c r="G26" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="H26">
-        <v>2008</v>
+        <v>2010</v>
       </c>
       <c r="I26" s="1">
-        <v>39525</v>
+        <v>40248</v>
       </c>
       <c r="J26" t="s">
-        <v>193</v>
+        <v>130</v>
       </c>
       <c r="K26" t="s">
         <v>43</v>
@@ -8224,51 +8300,51 @@
         <v>20</v>
       </c>
       <c r="M26" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="N26" t="s">
-        <v>304</v>
+        <v>319</v>
       </c>
       <c r="O26" t="s">
-        <v>360</v>
+        <v>345</v>
       </c>
       <c r="Q26">
-        <v>42.871989999999997</v>
+        <v>48.174337000000001</v>
       </c>
       <c r="R26">
-        <v>-73.226607000000001</v>
+        <v>-80.100126000000003</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>186</v>
       </c>
       <c r="B27" t="s">
-        <v>106</v>
+        <v>187</v>
       </c>
       <c r="C27" t="s">
-        <v>105</v>
+        <v>186</v>
       </c>
       <c r="D27" s="5">
-        <v>5755634</v>
+        <v>6011473</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>107</v>
+        <v>188</v>
       </c>
       <c r="F27" t="s">
         <v>51</v>
       </c>
       <c r="G27" t="s">
-        <v>108</v>
+        <v>189</v>
       </c>
       <c r="H27">
-        <v>2008</v>
-      </c>
-      <c r="I27">
-        <v>2008</v>
+        <v>2010</v>
+      </c>
+      <c r="I27" s="1">
+        <v>40242</v>
       </c>
       <c r="J27" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
       <c r="K27" t="s">
         <v>43</v>
@@ -8280,60 +8356,48 @@
         <v>298</v>
       </c>
       <c r="N27" t="s">
-        <v>299</v>
+        <v>354</v>
       </c>
       <c r="O27" t="s">
-        <v>300</v>
-      </c>
-      <c r="P27" t="s">
-        <v>406</v>
+        <v>366</v>
       </c>
       <c r="Q27">
-        <v>41.844515371877698</v>
+        <v>36.555458999999999</v>
       </c>
       <c r="R27">
-        <v>-74.098548155198898</v>
-      </c>
-      <c r="S27" t="s">
-        <v>415</v>
-      </c>
-      <c r="U27" t="s">
-        <v>325</v>
-      </c>
-      <c r="V27" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+        <v>-87.304068999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>122</v>
+        <v>189</v>
       </c>
       <c r="B28" t="s">
-        <v>123</v>
+        <v>190</v>
       </c>
       <c r="C28" t="s">
-        <v>122</v>
+        <v>189</v>
       </c>
       <c r="D28" s="5">
-        <v>1952982</v>
+        <v>6011474</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>124</v>
+        <v>191</v>
       </c>
       <c r="F28" t="s">
         <v>51</v>
       </c>
       <c r="G28" t="s">
-        <v>125</v>
+        <v>192</v>
       </c>
       <c r="H28">
         <v>2008</v>
       </c>
-      <c r="I28">
-        <v>2008</v>
+      <c r="I28" s="1">
+        <v>39525</v>
       </c>
       <c r="J28" t="s">
-        <v>117</v>
+        <v>193</v>
       </c>
       <c r="K28" t="s">
         <v>43</v>
@@ -8345,66 +8409,48 @@
         <v>298</v>
       </c>
       <c r="N28" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="O28" t="s">
-        <v>328</v>
+        <v>360</v>
       </c>
       <c r="Q28">
-        <v>41.844515371877698</v>
+        <v>42.871989999999997</v>
       </c>
       <c r="R28">
-        <v>-74.098548155198898</v>
-      </c>
-      <c r="S28" t="s">
-        <v>379</v>
-      </c>
-      <c r="T28" t="s">
-        <v>380</v>
-      </c>
-      <c r="U28" t="s">
-        <v>378</v>
-      </c>
-      <c r="V28" t="s">
-        <v>384</v>
-      </c>
-      <c r="W28" s="6" t="s">
-        <v>386</v>
-      </c>
-      <c r="X28" s="2" t="s">
-        <v>387</v>
+        <v>-73.226607000000001</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="B29" t="s">
-        <v>221</v>
+        <v>194</v>
       </c>
       <c r="C29" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="D29" s="5">
-        <v>6011481</v>
+        <v>6011475</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>222</v>
+        <v>195</v>
       </c>
       <c r="F29" t="s">
         <v>51</v>
       </c>
       <c r="G29" t="s">
-        <v>223</v>
+        <v>196</v>
       </c>
       <c r="H29">
         <v>2009</v>
       </c>
       <c r="I29" s="1">
-        <v>39882</v>
+        <v>39840</v>
       </c>
       <c r="J29" t="s">
-        <v>193</v>
+        <v>130</v>
       </c>
       <c r="K29" t="s">
         <v>43</v>
@@ -8416,45 +8462,45 @@
         <v>298</v>
       </c>
       <c r="N29" t="s">
-        <v>299</v>
+        <v>349</v>
       </c>
       <c r="O29" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="Q29">
-        <v>41.949971359391597</v>
+        <v>41.745700999999997</v>
       </c>
       <c r="R29">
-        <v>-74.288489118822994</v>
+        <v>-73.158473999999998</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
       <c r="B30" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="C30" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
       <c r="D30" s="5">
-        <v>6011470</v>
+        <v>6011476</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>179</v>
+        <v>198</v>
       </c>
       <c r="F30" t="s">
         <v>51</v>
       </c>
       <c r="G30" t="s">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="H30">
         <v>2009</v>
       </c>
       <c r="I30" s="1">
-        <v>39990</v>
+        <v>39875</v>
       </c>
       <c r="J30" t="s">
         <v>130</v>
@@ -8469,48 +8515,48 @@
         <v>298</v>
       </c>
       <c r="N30" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="O30" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="Q30">
-        <v>40.877385651285401</v>
+        <v>37.322156999999997</v>
       </c>
       <c r="R30">
-        <v>-74.968855407371393</v>
+        <v>-80.756189000000006</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>258</v>
+        <v>199</v>
       </c>
       <c r="B31" t="s">
-        <v>259</v>
+        <v>200</v>
       </c>
       <c r="C31" t="s">
-        <v>258</v>
+        <v>199</v>
       </c>
       <c r="D31" s="5">
-        <v>6011494</v>
+        <v>6011477</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>260</v>
+        <v>201</v>
       </c>
       <c r="F31" t="s">
-        <v>232</v>
+        <v>51</v>
       </c>
       <c r="G31" t="s">
-        <v>257</v>
+        <v>202</v>
       </c>
       <c r="H31">
-        <v>2012</v>
+        <v>2008</v>
       </c>
       <c r="I31" s="1">
-        <v>40969</v>
+        <v>39528</v>
       </c>
       <c r="J31" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="K31" t="s">
         <v>43</v>
@@ -8522,51 +8568,51 @@
         <v>298</v>
       </c>
       <c r="N31" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="O31" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="Q31">
-        <v>39.838700000000003</v>
+        <v>42.592351000000001</v>
       </c>
       <c r="R31">
-        <v>-75.563800000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
+        <v>-73.226241999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>174</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>175</v>
+        <v>203</v>
       </c>
       <c r="C32" t="s">
-        <v>174</v>
+        <v>41</v>
       </c>
       <c r="D32" s="5">
-        <v>6011469</v>
+        <v>3545532</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>176</v>
+        <v>204</v>
       </c>
       <c r="F32" t="s">
         <v>51</v>
       </c>
       <c r="G32" t="s">
-        <v>177</v>
+        <v>205</v>
       </c>
       <c r="H32">
-        <v>2009</v>
-      </c>
-      <c r="I32" s="1">
-        <v>39897</v>
+        <v>2015</v>
+      </c>
+      <c r="I32">
+        <v>2015</v>
       </c>
       <c r="J32" t="s">
-        <v>130</v>
+        <v>18</v>
       </c>
       <c r="K32" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="L32" t="s">
         <v>20</v>
@@ -8575,51 +8621,60 @@
         <v>298</v>
       </c>
       <c r="N32" t="s">
-        <v>339</v>
+        <v>310</v>
       </c>
       <c r="O32" t="s">
-        <v>340</v>
+        <v>311</v>
+      </c>
+      <c r="P32" t="s">
+        <v>407</v>
       </c>
       <c r="Q32">
-        <v>40.888610999999997</v>
+        <v>34.574328000000001</v>
       </c>
       <c r="R32">
-        <v>-77.386111</v>
-      </c>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
+        <v>-86.220834999999994</v>
+      </c>
+      <c r="W32" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="X32" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>208</v>
+        <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="C33" t="s">
-        <v>208</v>
+        <v>47</v>
       </c>
       <c r="D33" s="5">
-        <v>6011480</v>
+        <v>3545533</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="F33" t="s">
         <v>51</v>
       </c>
       <c r="G33" t="s">
-        <v>129</v>
+        <v>208</v>
       </c>
       <c r="H33">
-        <v>2010</v>
-      </c>
-      <c r="I33" s="1">
-        <v>40242</v>
+        <v>2016</v>
+      </c>
+      <c r="I33">
+        <v>2016</v>
       </c>
       <c r="J33" t="s">
-        <v>130</v>
+        <v>18</v>
       </c>
       <c r="K33" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="L33" t="s">
         <v>20</v>
@@ -8628,48 +8683,54 @@
         <v>298</v>
       </c>
       <c r="N33" t="s">
-        <v>355</v>
+        <v>312</v>
       </c>
       <c r="O33" t="s">
-        <v>367</v>
+        <v>313</v>
+      </c>
+      <c r="P33" t="s">
+        <v>406</v>
       </c>
       <c r="Q33">
-        <v>39.69717</v>
+        <v>47.550894599999999</v>
       </c>
       <c r="R33">
-        <v>-78.820670000000007</v>
-      </c>
-      <c r="X33" s="9" t="s">
-        <v>417</v>
+        <v>-121.53941880000001</v>
+      </c>
+      <c r="W33" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="X33" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>180</v>
+        <v>202</v>
       </c>
       <c r="B34" t="s">
-        <v>181</v>
+        <v>213</v>
       </c>
       <c r="C34" t="s">
-        <v>180</v>
+        <v>202</v>
       </c>
       <c r="D34" s="5">
-        <v>6011471</v>
+        <v>6011478</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>182</v>
+        <v>214</v>
       </c>
       <c r="F34" t="s">
         <v>51</v>
       </c>
       <c r="G34" t="s">
-        <v>183</v>
+        <v>215</v>
       </c>
       <c r="H34">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="I34" s="1">
-        <v>39843</v>
+        <v>39539</v>
       </c>
       <c r="J34" t="s">
         <v>130</v>
@@ -8684,48 +8745,48 @@
         <v>298</v>
       </c>
       <c r="N34" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="O34" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="Q34">
-        <v>38.664935999999997</v>
+        <v>41.745700999999997</v>
       </c>
       <c r="R34">
-        <v>-79.430160999999998</v>
+        <v>-73.158473999999998</v>
       </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>273</v>
+        <v>205</v>
       </c>
       <c r="B35" t="s">
-        <v>274</v>
+        <v>216</v>
       </c>
       <c r="C35" t="s">
-        <v>273</v>
+        <v>205</v>
       </c>
       <c r="D35" s="5">
-        <v>11812088</v>
+        <v>6011479</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>275</v>
+        <v>217</v>
       </c>
       <c r="F35" t="s">
         <v>51</v>
       </c>
       <c r="G35" t="s">
-        <v>276</v>
+        <v>218</v>
       </c>
       <c r="H35">
-        <v>2014</v>
-      </c>
-      <c r="I35">
-        <v>2014</v>
+        <v>2010</v>
+      </c>
+      <c r="I35" s="1">
+        <v>40217</v>
       </c>
       <c r="J35" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="K35" t="s">
         <v>43</v>
@@ -8734,48 +8795,48 @@
         <v>20</v>
       </c>
       <c r="M35" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="N35" t="s">
-        <v>319</v>
+        <v>354</v>
       </c>
       <c r="O35" t="s">
-        <v>334</v>
+        <v>365</v>
       </c>
       <c r="Q35">
-        <v>43.468915000000003</v>
+        <v>36.509321</v>
       </c>
       <c r="R35">
-        <v>-79.911533000000006</v>
+        <v>-82.328933000000006</v>
       </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>183</v>
+        <v>208</v>
       </c>
       <c r="B36" t="s">
-        <v>184</v>
+        <v>219</v>
       </c>
       <c r="C36" t="s">
-        <v>183</v>
+        <v>208</v>
       </c>
       <c r="D36" s="5">
-        <v>6011472</v>
+        <v>6011480</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>185</v>
+        <v>220</v>
       </c>
       <c r="F36" t="s">
         <v>51</v>
       </c>
       <c r="G36" t="s">
-        <v>186</v>
+        <v>129</v>
       </c>
       <c r="H36">
         <v>2010</v>
       </c>
       <c r="I36" s="1">
-        <v>40248</v>
+        <v>40242</v>
       </c>
       <c r="J36" t="s">
         <v>130</v>
@@ -8787,51 +8848,54 @@
         <v>20</v>
       </c>
       <c r="M36" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="N36" t="s">
-        <v>319</v>
+        <v>355</v>
       </c>
       <c r="O36" t="s">
-        <v>345</v>
+        <v>367</v>
       </c>
       <c r="Q36">
-        <v>48.174337000000001</v>
+        <v>39.69717</v>
       </c>
       <c r="R36">
-        <v>-80.100126000000003</v>
+        <v>-78.820670000000007</v>
+      </c>
+      <c r="X36" s="9" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>138</v>
+        <v>212</v>
       </c>
       <c r="B37" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="C37" t="s">
-        <v>138</v>
+        <v>212</v>
       </c>
       <c r="D37" s="5">
-        <v>6011483</v>
+        <v>6011481</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="F37" t="s">
         <v>51</v>
       </c>
       <c r="G37" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="H37">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="I37" s="1">
-        <v>40252</v>
+        <v>39882</v>
       </c>
       <c r="J37" t="s">
-        <v>130</v>
+        <v>193</v>
       </c>
       <c r="K37" t="s">
         <v>43</v>
@@ -8840,48 +8904,48 @@
         <v>20</v>
       </c>
       <c r="M37" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="N37" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="O37" t="s">
-        <v>305</v>
+        <v>353</v>
       </c>
       <c r="Q37">
-        <v>48.174337000000001</v>
+        <v>41.949971359391597</v>
       </c>
       <c r="R37">
-        <v>-80.100126000000003</v>
+        <v>-74.288489118822994</v>
       </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>196</v>
+        <v>134</v>
       </c>
       <c r="B38" t="s">
-        <v>197</v>
+        <v>224</v>
       </c>
       <c r="C38" t="s">
-        <v>196</v>
+        <v>134</v>
       </c>
       <c r="D38" s="5">
-        <v>6011476</v>
+        <v>6011482</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>198</v>
+        <v>225</v>
       </c>
       <c r="F38" t="s">
         <v>51</v>
       </c>
       <c r="G38" t="s">
-        <v>199</v>
+        <v>226</v>
       </c>
       <c r="H38">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="I38" s="1">
-        <v>39875</v>
+        <v>40205</v>
       </c>
       <c r="J38" t="s">
         <v>130</v>
@@ -8896,45 +8960,45 @@
         <v>298</v>
       </c>
       <c r="N38" t="s">
-        <v>351</v>
+        <v>304</v>
       </c>
       <c r="O38" t="s">
-        <v>352</v>
+        <v>364</v>
       </c>
       <c r="Q38">
-        <v>37.322156999999997</v>
+        <v>43.451169999999998</v>
       </c>
       <c r="R38">
-        <v>-80.756189000000006</v>
+        <v>-72.942554999999999</v>
       </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>205</v>
+        <v>138</v>
       </c>
       <c r="B39" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
       <c r="C39" t="s">
-        <v>205</v>
+        <v>138</v>
       </c>
       <c r="D39" s="5">
-        <v>6011479</v>
+        <v>6011483</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
       <c r="F39" t="s">
         <v>51</v>
       </c>
       <c r="G39" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="H39">
         <v>2010</v>
       </c>
       <c r="I39" s="1">
-        <v>40217</v>
+        <v>40252</v>
       </c>
       <c r="J39" t="s">
         <v>130</v>
@@ -8946,36 +9010,36 @@
         <v>20</v>
       </c>
       <c r="M39" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="N39" t="s">
-        <v>354</v>
+        <v>319</v>
       </c>
       <c r="O39" t="s">
-        <v>365</v>
+        <v>305</v>
       </c>
       <c r="Q39">
-        <v>36.509321</v>
+        <v>48.174337000000001</v>
       </c>
       <c r="R39">
-        <v>-82.328933000000006</v>
+        <v>-80.100126000000003</v>
       </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>246</v>
+        <v>142</v>
       </c>
       <c r="B40" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
       <c r="C40" t="s">
-        <v>246</v>
+        <v>142</v>
       </c>
       <c r="D40" s="5">
-        <v>6011490</v>
+        <v>6011484</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>248</v>
+        <v>231</v>
       </c>
       <c r="F40" t="s">
         <v>232</v>
@@ -8984,10 +9048,10 @@
         <v>233</v>
       </c>
       <c r="H40">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="I40" s="1">
-        <v>40590</v>
+        <v>40275</v>
       </c>
       <c r="J40" t="s">
         <v>130</v>
@@ -9002,45 +9066,45 @@
         <v>298</v>
       </c>
       <c r="N40" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="O40" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="Q40">
-        <v>36.968234063873403</v>
+        <v>36.465316000000001</v>
       </c>
       <c r="R40">
-        <v>-82.639469435652799</v>
+        <v>-84.971273999999994</v>
       </c>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>142</v>
+        <v>157</v>
       </c>
       <c r="B41" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
       <c r="C41" t="s">
-        <v>142</v>
+        <v>157</v>
       </c>
       <c r="D41" s="5">
-        <v>6011484</v>
+        <v>6011488</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="F41" t="s">
         <v>232</v>
       </c>
       <c r="G41" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
       <c r="H41">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="I41" s="1">
-        <v>40275</v>
+        <v>41011</v>
       </c>
       <c r="J41" t="s">
         <v>130</v>
@@ -9052,54 +9116,54 @@
         <v>20</v>
       </c>
       <c r="M41" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="N41" t="s">
-        <v>354</v>
+        <v>292</v>
       </c>
       <c r="O41" t="s">
-        <v>368</v>
+        <v>297</v>
       </c>
       <c r="Q41">
-        <v>36.465316000000001</v>
+        <v>45.93694</v>
       </c>
       <c r="R41">
-        <v>-84.971273999999994</v>
-      </c>
-    </row>
-    <row r="42" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+        <v>-64.476939999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>161</v>
       </c>
       <c r="B42" t="s">
-        <v>203</v>
+        <v>244</v>
       </c>
       <c r="C42" t="s">
-        <v>41</v>
+        <v>161</v>
       </c>
       <c r="D42" s="5">
-        <v>3545532</v>
+        <v>6011489</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>204</v>
+        <v>245</v>
       </c>
       <c r="F42" t="s">
-        <v>51</v>
+        <v>232</v>
       </c>
       <c r="G42" t="s">
-        <v>205</v>
+        <v>233</v>
       </c>
       <c r="H42">
-        <v>2015</v>
-      </c>
-      <c r="I42">
-        <v>2015</v>
+        <v>2012</v>
+      </c>
+      <c r="I42" s="1">
+        <v>40987</v>
       </c>
       <c r="J42" t="s">
-        <v>18</v>
+        <v>117</v>
       </c>
       <c r="K42" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="L42" t="s">
         <v>20</v>
@@ -9108,57 +9172,48 @@
         <v>298</v>
       </c>
       <c r="N42" t="s">
-        <v>310</v>
+        <v>359</v>
       </c>
       <c r="O42" t="s">
-        <v>311</v>
-      </c>
-      <c r="P42" t="s">
-        <v>407</v>
+        <v>374</v>
       </c>
       <c r="Q42">
-        <v>34.574328000000001</v>
+        <v>39.048609999999996</v>
       </c>
       <c r="R42">
-        <v>-86.220834999999994</v>
-      </c>
-      <c r="W42" s="6" t="s">
-        <v>408</v>
-      </c>
-      <c r="X42" t="s">
-        <v>410</v>
+        <v>-90.88167</v>
       </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="B43" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C43" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="D43" s="5">
-        <v>6011493</v>
+        <v>6011490</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F43" t="s">
         <v>232</v>
       </c>
       <c r="G43" t="s">
-        <v>257</v>
+        <v>233</v>
       </c>
       <c r="H43">
         <v>2011</v>
       </c>
       <c r="I43" s="1">
-        <v>40566</v>
+        <v>40590</v>
       </c>
       <c r="J43" t="s">
-        <v>193</v>
+        <v>130</v>
       </c>
       <c r="K43" t="s">
         <v>43</v>
@@ -9170,45 +9225,45 @@
         <v>298</v>
       </c>
       <c r="N43" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="O43" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="Q43">
-        <v>38.702026438267701</v>
+        <v>36.968234063873403</v>
       </c>
       <c r="R43">
-        <v>-86.233603821942907</v>
+        <v>-82.639469435652799</v>
       </c>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>251</v>
+        <v>164</v>
       </c>
       <c r="B44" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C44" t="s">
-        <v>251</v>
+        <v>164</v>
       </c>
       <c r="D44" s="5">
-        <v>6011492</v>
+        <v>6011491</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F44" t="s">
         <v>232</v>
       </c>
       <c r="G44" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="H44">
         <v>2011</v>
       </c>
       <c r="I44" s="1">
-        <v>40572</v>
+        <v>40583</v>
       </c>
       <c r="J44" t="s">
         <v>130</v>
@@ -9223,45 +9278,45 @@
         <v>298</v>
       </c>
       <c r="N44" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="O44" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="Q44">
-        <v>38.229909999999997</v>
+        <v>36.555458999999999</v>
       </c>
       <c r="R44">
-        <v>-86.294910000000002</v>
+        <v>-87.304068999999998</v>
       </c>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>186</v>
+        <v>251</v>
       </c>
       <c r="B45" t="s">
-        <v>187</v>
+        <v>252</v>
       </c>
       <c r="C45" t="s">
-        <v>186</v>
+        <v>251</v>
       </c>
       <c r="D45" s="5">
-        <v>6011473</v>
+        <v>6011492</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>188</v>
+        <v>253</v>
       </c>
       <c r="F45" t="s">
-        <v>51</v>
+        <v>232</v>
       </c>
       <c r="G45" t="s">
-        <v>189</v>
+        <v>243</v>
       </c>
       <c r="H45">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="I45" s="1">
-        <v>40242</v>
+        <v>40572</v>
       </c>
       <c r="J45" t="s">
         <v>130</v>
@@ -9276,48 +9331,48 @@
         <v>298</v>
       </c>
       <c r="N45" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="O45" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="Q45">
-        <v>36.555458999999999</v>
+        <v>38.229909999999997</v>
       </c>
       <c r="R45">
-        <v>-87.304068999999998</v>
+        <v>-86.294910000000002</v>
       </c>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>164</v>
+        <v>254</v>
       </c>
       <c r="B46" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="C46" t="s">
-        <v>164</v>
+        <v>254</v>
       </c>
       <c r="D46" s="5">
-        <v>6011491</v>
+        <v>6011493</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="F46" t="s">
         <v>232</v>
       </c>
       <c r="G46" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
       <c r="H46">
         <v>2011</v>
       </c>
       <c r="I46" s="1">
-        <v>40583</v>
+        <v>40566</v>
       </c>
       <c r="J46" t="s">
-        <v>130</v>
+        <v>193</v>
       </c>
       <c r="K46" t="s">
         <v>43</v>
@@ -9329,48 +9384,48 @@
         <v>298</v>
       </c>
       <c r="N46" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="O46" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="Q46">
-        <v>36.555458999999999</v>
+        <v>38.702026438267701</v>
       </c>
       <c r="R46">
-        <v>-87.304068999999998</v>
-      </c>
-    </row>
-    <row r="47" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+        <v>-86.233603821942907</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>38</v>
+        <v>258</v>
       </c>
       <c r="B47" t="s">
-        <v>39</v>
+        <v>259</v>
       </c>
       <c r="C47" t="s">
-        <v>38</v>
+        <v>258</v>
       </c>
       <c r="D47" s="5">
-        <v>5755618</v>
+        <v>6011494</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>40</v>
+        <v>260</v>
       </c>
       <c r="F47" t="s">
-        <v>16</v>
+        <v>232</v>
       </c>
       <c r="G47" t="s">
-        <v>41</v>
+        <v>257</v>
       </c>
       <c r="H47">
-        <v>2015</v>
-      </c>
-      <c r="I47">
-        <v>2015</v>
+        <v>2012</v>
+      </c>
+      <c r="I47" s="1">
+        <v>40969</v>
       </c>
       <c r="J47" t="s">
-        <v>42</v>
+        <v>117</v>
       </c>
       <c r="K47" t="s">
         <v>43</v>
@@ -9379,69 +9434,51 @@
         <v>20</v>
       </c>
       <c r="M47" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="N47" t="s">
-        <v>319</v>
+        <v>358</v>
       </c>
       <c r="O47" t="s">
-        <v>320</v>
-      </c>
-      <c r="P47" t="s">
-        <v>406</v>
+        <v>373</v>
       </c>
       <c r="Q47">
-        <v>48.498627856338103</v>
+        <v>39.838700000000003</v>
       </c>
       <c r="R47">
-        <v>-89.227383734950806</v>
-      </c>
-      <c r="S47" t="s">
-        <v>415</v>
-      </c>
-      <c r="T47" t="s">
-        <v>414</v>
-      </c>
-      <c r="U47" t="s">
-        <v>321</v>
-      </c>
-      <c r="V47" t="s">
-        <v>412</v>
-      </c>
-      <c r="W47" s="2" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="48" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+        <v>-75.563800000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>44</v>
+        <v>215</v>
       </c>
       <c r="B48" t="s">
-        <v>45</v>
+        <v>261</v>
       </c>
       <c r="C48" t="s">
-        <v>44</v>
+        <v>215</v>
       </c>
       <c r="D48" s="5">
-        <v>5755619</v>
+        <v>6011495</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>46</v>
+        <v>262</v>
       </c>
       <c r="F48" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="G48" t="s">
-        <v>47</v>
+        <v>263</v>
       </c>
       <c r="H48">
-        <v>2015</v>
-      </c>
-      <c r="I48">
-        <v>2015</v>
+        <v>2011</v>
+      </c>
+      <c r="I48" s="1">
+        <v>40889</v>
       </c>
       <c r="J48" t="s">
-        <v>42</v>
+        <v>117</v>
       </c>
       <c r="K48" t="s">
         <v>43</v>
@@ -9450,69 +9487,54 @@
         <v>20</v>
       </c>
       <c r="M48" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="N48" t="s">
-        <v>319</v>
+        <v>357</v>
       </c>
       <c r="O48" t="s">
-        <v>320</v>
-      </c>
-      <c r="P48" t="s">
-        <v>406</v>
+        <v>372</v>
       </c>
       <c r="Q48">
-        <v>48.498627856338103</v>
+        <v>44.349651999999999</v>
       </c>
       <c r="R48">
-        <v>-89.227383734950806</v>
-      </c>
-      <c r="S48" t="s">
-        <v>415</v>
-      </c>
-      <c r="T48" t="s">
-        <v>414</v>
-      </c>
-      <c r="U48" t="s">
-        <v>321</v>
-      </c>
-      <c r="V48" t="s">
-        <v>413</v>
-      </c>
-      <c r="W48" s="2" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
+        <v>-68.211070000000007</v>
+      </c>
+      <c r="X48" s="9" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>61</v>
+        <v>273</v>
       </c>
       <c r="B49" t="s">
-        <v>62</v>
+        <v>274</v>
       </c>
       <c r="C49" t="s">
-        <v>61</v>
+        <v>273</v>
       </c>
       <c r="D49" s="5">
-        <v>5755623</v>
+        <v>11812088</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>63</v>
+        <v>275</v>
       </c>
       <c r="F49" t="s">
         <v>51</v>
       </c>
       <c r="G49" t="s">
-        <v>64</v>
+        <v>276</v>
       </c>
       <c r="H49">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="I49">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="J49" t="s">
-        <v>42</v>
+        <v>117</v>
       </c>
       <c r="K49" t="s">
         <v>43</v>
@@ -9527,107 +9549,95 @@
         <v>319</v>
       </c>
       <c r="O49" t="s">
-        <v>320</v>
+        <v>334</v>
       </c>
       <c r="Q49">
-        <v>48.498627856338103</v>
+        <v>43.468915000000003</v>
       </c>
       <c r="R49">
-        <v>-89.227383734950806</v>
-      </c>
-      <c r="U49" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="50" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+        <v>-79.911533000000006</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>277</v>
       </c>
       <c r="B50" t="s">
-        <v>14</v>
+        <v>278</v>
       </c>
       <c r="C50" t="s">
-        <v>13</v>
+        <v>277</v>
       </c>
       <c r="D50" s="5">
-        <v>3545531</v>
+        <v>11812089</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>15</v>
+        <v>279</v>
       </c>
       <c r="F50" t="s">
+        <v>51</v>
+      </c>
+      <c r="G50" t="s">
+        <v>280</v>
+      </c>
+      <c r="H50">
+        <v>2013</v>
+      </c>
+      <c r="I50">
+        <v>2013</v>
+      </c>
+      <c r="J50" t="s">
+        <v>117</v>
+      </c>
+      <c r="K50" t="s">
+        <v>43</v>
+      </c>
+      <c r="L50" t="s">
+        <v>20</v>
+      </c>
+      <c r="M50" t="s">
+        <v>291</v>
+      </c>
+      <c r="N50" t="s">
+        <v>322</v>
+      </c>
+      <c r="O50" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q50">
+        <v>44.992969000000002</v>
+      </c>
+      <c r="R50">
+        <v>-64.167955000000006</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>281</v>
+      </c>
+      <c r="B51" t="s">
+        <v>282</v>
+      </c>
+      <c r="C51" t="s">
+        <v>281</v>
+      </c>
+      <c r="D51" s="5">
+        <v>11812090</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="F51" t="s">
         <v>16</v>
       </c>
-      <c r="G50" t="s">
-        <v>17</v>
-      </c>
-      <c r="H50">
-        <v>2016</v>
-      </c>
-      <c r="I50">
-        <v>2016</v>
-      </c>
-      <c r="J50" t="s">
-        <v>18</v>
-      </c>
-      <c r="K50" t="s">
-        <v>19</v>
-      </c>
-      <c r="L50" t="s">
-        <v>20</v>
-      </c>
-      <c r="M50" t="s">
-        <v>298</v>
-      </c>
-      <c r="N50" t="s">
-        <v>302</v>
-      </c>
-      <c r="O50" t="s">
-        <v>309</v>
-      </c>
-      <c r="P50" t="s">
-        <v>406</v>
-      </c>
-      <c r="Q50" s="8">
-        <v>43.0274</v>
-      </c>
-      <c r="R50" s="8">
-        <v>-90.092200000000005</v>
-      </c>
-      <c r="W50" s="6" t="s">
-        <v>408</v>
-      </c>
-      <c r="X50" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>161</v>
-      </c>
-      <c r="B51" t="s">
-        <v>244</v>
-      </c>
-      <c r="C51" t="s">
-        <v>161</v>
-      </c>
-      <c r="D51" s="5">
-        <v>6011489</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="F51" t="s">
-        <v>232</v>
-      </c>
       <c r="G51" t="s">
-        <v>233</v>
+        <v>284</v>
       </c>
       <c r="H51">
         <v>2012</v>
       </c>
       <c r="I51" s="1">
-        <v>40987</v>
+        <v>40967</v>
       </c>
       <c r="J51" t="s">
         <v>117</v>
@@ -9639,92 +9649,83 @@
         <v>20</v>
       </c>
       <c r="M51" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="N51" t="s">
-        <v>359</v>
+        <v>292</v>
       </c>
       <c r="O51" t="s">
-        <v>374</v>
+        <v>332</v>
       </c>
       <c r="Q51">
-        <v>39.048609999999996</v>
+        <v>45.300289999999997</v>
       </c>
       <c r="R51">
-        <v>-90.88167</v>
-      </c>
-    </row>
-    <row r="52" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+        <v>-66.050550000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>47</v>
+        <v>285</v>
       </c>
       <c r="B52" t="s">
-        <v>206</v>
+        <v>286</v>
       </c>
       <c r="C52" t="s">
-        <v>47</v>
+        <v>285</v>
       </c>
       <c r="D52" s="5">
-        <v>3545533</v>
+        <v>11812091</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>207</v>
+        <v>287</v>
       </c>
       <c r="F52" t="s">
         <v>51</v>
       </c>
       <c r="G52" t="s">
-        <v>208</v>
+        <v>288</v>
       </c>
       <c r="H52">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="I52">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="J52" t="s">
-        <v>18</v>
+        <v>117</v>
       </c>
       <c r="K52" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="L52" t="s">
         <v>20</v>
       </c>
       <c r="M52" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="N52" t="s">
-        <v>312</v>
+        <v>292</v>
       </c>
       <c r="O52" t="s">
-        <v>313</v>
-      </c>
-      <c r="P52" t="s">
-        <v>406</v>
+        <v>297</v>
       </c>
       <c r="Q52">
-        <v>47.550894599999999</v>
+        <v>45.93694</v>
       </c>
       <c r="R52">
-        <v>-121.53941880000001</v>
-      </c>
-      <c r="W52" s="6" t="s">
-        <v>408</v>
-      </c>
-      <c r="X52" t="s">
-        <v>411</v>
+        <v>-64.476939999999999</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="W28" r:id="rId1" xr:uid="{70AAB464-2D71-FD4F-8671-23385CED9FD3}"/>
-    <hyperlink ref="W50" r:id="rId2" display="https://doi.org/10.1038/s41467-017-02441-z" xr:uid="{5795B073-C652-F844-B0C9-802D2615ACCB}"/>
-    <hyperlink ref="W50" r:id="rId3" xr:uid="{0F40B4A2-965F-3642-9EF7-F6435E9BDD31}"/>
-    <hyperlink ref="W42" r:id="rId4" xr:uid="{41A233D3-D3A2-654A-A79A-8995C2D847F0}"/>
-    <hyperlink ref="W52" r:id="rId5" xr:uid="{EA316F4B-52D4-ED48-8493-838FD348465B}"/>
-    <hyperlink ref="X33" r:id="rId6" location="close --&gt; used to find  most clustered group of caves in the county" xr:uid="{D4ACC45F-471F-4740-9C90-37B3D50FF8DD}"/>
-    <hyperlink ref="X21" r:id="rId7" xr:uid="{787EAAA7-7854-7248-B070-6066565116D2}"/>
+    <hyperlink ref="W22" r:id="rId1" xr:uid="{70AAB464-2D71-FD4F-8671-23385CED9FD3}"/>
+    <hyperlink ref="W2" r:id="rId2" display="https://doi.org/10.1038/s41467-017-02441-z" xr:uid="{5795B073-C652-F844-B0C9-802D2615ACCB}"/>
+    <hyperlink ref="W2" r:id="rId3" xr:uid="{0F40B4A2-965F-3642-9EF7-F6435E9BDD31}"/>
+    <hyperlink ref="W32" r:id="rId4" xr:uid="{41A233D3-D3A2-654A-A79A-8995C2D847F0}"/>
+    <hyperlink ref="W33" r:id="rId5" xr:uid="{EA316F4B-52D4-ED48-8493-838FD348465B}"/>
+    <hyperlink ref="X36" r:id="rId6" location="close --&gt; used to find  most clustered group of caves in the county" xr:uid="{D4ACC45F-471F-4740-9C90-37B3D50FF8DD}"/>
+    <hyperlink ref="X48" r:id="rId7" xr:uid="{787EAAA7-7854-7248-B070-6066565116D2}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -9739,7 +9740,7 @@
   <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10320,4 +10321,581 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76291800-C65C-8C4F-9D97-BB7E20AAC35D}">
+  <dimension ref="A1:C51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B1" t="s">
+        <v>420</v>
+      </c>
+      <c r="C1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>-90.092200000000005</v>
+      </c>
+      <c r="C2">
+        <v>43.0274</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3">
+        <v>-89.227383734950806</v>
+      </c>
+      <c r="C3">
+        <v>48.498627856338103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4">
+        <v>-89.227383734950806</v>
+      </c>
+      <c r="C4">
+        <v>48.498627856338103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5">
+        <v>-63.830206168139703</v>
+      </c>
+      <c r="C5">
+        <v>45.003125911591702</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6">
+        <v>-63.830206168139703</v>
+      </c>
+      <c r="C6">
+        <v>45.003125911591702</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7">
+        <v>-62.618592999999997</v>
+      </c>
+      <c r="C7">
+        <v>46.011941999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8">
+        <v>-89.227383734950806</v>
+      </c>
+      <c r="C8">
+        <v>48.498627856338103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9">
+        <v>-64.671137999999999</v>
+      </c>
+      <c r="C9">
+        <v>45.913153999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10">
+        <v>-65.610500000000002</v>
+      </c>
+      <c r="C10">
+        <v>45.8172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11">
+        <v>-65.610500000000002</v>
+      </c>
+      <c r="C11">
+        <v>45.8172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12">
+        <v>-64.671137999999999</v>
+      </c>
+      <c r="C12">
+        <v>45.913153999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13">
+        <v>-65.439909999999998</v>
+      </c>
+      <c r="C13">
+        <v>45.615960000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14">
+        <v>-64.476939999999999</v>
+      </c>
+      <c r="C14">
+        <v>45.93694</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15">
+        <v>-65.439909999999998</v>
+      </c>
+      <c r="C15">
+        <v>45.615960000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16">
+        <v>-65.439909999999998</v>
+      </c>
+      <c r="C16">
+        <v>45.615960000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17">
+        <v>-65.610500000000002</v>
+      </c>
+      <c r="C17">
+        <v>45.8172</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18">
+        <v>-74.098548155198898</v>
+      </c>
+      <c r="C18">
+        <v>41.844515371877698</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19">
+        <v>-64.671137999999999</v>
+      </c>
+      <c r="C19">
+        <v>45.913153999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20">
+        <v>-64.476939999999999</v>
+      </c>
+      <c r="C20">
+        <v>45.93694</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21">
+        <v>-62.618592999999997</v>
+      </c>
+      <c r="C21">
+        <v>46.011941999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>123</v>
+      </c>
+      <c r="B22">
+        <v>-74.098548155198898</v>
+      </c>
+      <c r="C22">
+        <v>41.844515371877698</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>175</v>
+      </c>
+      <c r="B23">
+        <v>-77.386111</v>
+      </c>
+      <c r="C23">
+        <v>40.888610999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>178</v>
+      </c>
+      <c r="B24">
+        <v>-74.968855407371393</v>
+      </c>
+      <c r="C24">
+        <v>40.877385651285401</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>181</v>
+      </c>
+      <c r="B25">
+        <v>-79.430160999999998</v>
+      </c>
+      <c r="C25">
+        <v>38.664935999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>184</v>
+      </c>
+      <c r="B26">
+        <v>-80.100126000000003</v>
+      </c>
+      <c r="C26">
+        <v>48.174337000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>187</v>
+      </c>
+      <c r="B27">
+        <v>-87.304068999999998</v>
+      </c>
+      <c r="C27">
+        <v>36.555458999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>190</v>
+      </c>
+      <c r="B28">
+        <v>-73.226607000000001</v>
+      </c>
+      <c r="C28">
+        <v>42.871989999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>194</v>
+      </c>
+      <c r="B29">
+        <v>-73.158473999999998</v>
+      </c>
+      <c r="C29">
+        <v>41.745700999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>197</v>
+      </c>
+      <c r="B30">
+        <v>-80.756189000000006</v>
+      </c>
+      <c r="C30">
+        <v>37.322156999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>200</v>
+      </c>
+      <c r="B31">
+        <v>-73.226241999999999</v>
+      </c>
+      <c r="C31">
+        <v>42.592351000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>203</v>
+      </c>
+      <c r="B32">
+        <v>-86.220834999999994</v>
+      </c>
+      <c r="C32">
+        <v>34.574328000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>213</v>
+      </c>
+      <c r="B33">
+        <v>-73.158473999999998</v>
+      </c>
+      <c r="C33">
+        <v>41.745700999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>216</v>
+      </c>
+      <c r="B34">
+        <v>-82.328933000000006</v>
+      </c>
+      <c r="C34">
+        <v>36.509321</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>219</v>
+      </c>
+      <c r="B35">
+        <v>-78.820670000000007</v>
+      </c>
+      <c r="C35">
+        <v>39.69717</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>221</v>
+      </c>
+      <c r="B36">
+        <v>-74.288489118822994</v>
+      </c>
+      <c r="C36">
+        <v>41.949971359391597</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>224</v>
+      </c>
+      <c r="B37">
+        <v>-72.942554999999999</v>
+      </c>
+      <c r="C37">
+        <v>43.451169999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>227</v>
+      </c>
+      <c r="B38">
+        <v>-80.100126000000003</v>
+      </c>
+      <c r="C38">
+        <v>48.174337000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>230</v>
+      </c>
+      <c r="B39">
+        <v>-84.971273999999994</v>
+      </c>
+      <c r="C39">
+        <v>36.465316000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>241</v>
+      </c>
+      <c r="B40">
+        <v>-64.476939999999999</v>
+      </c>
+      <c r="C40">
+        <v>45.93694</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>244</v>
+      </c>
+      <c r="B41">
+        <v>-90.88167</v>
+      </c>
+      <c r="C41">
+        <v>39.048609999999996</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>247</v>
+      </c>
+      <c r="B42">
+        <v>-82.639469435652799</v>
+      </c>
+      <c r="C42">
+        <v>36.968234063873403</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>249</v>
+      </c>
+      <c r="B43">
+        <v>-87.304068999999998</v>
+      </c>
+      <c r="C43">
+        <v>36.555458999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>252</v>
+      </c>
+      <c r="B44">
+        <v>-86.294910000000002</v>
+      </c>
+      <c r="C44">
+        <v>38.229909999999997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>255</v>
+      </c>
+      <c r="B45">
+        <v>-86.233603821942907</v>
+      </c>
+      <c r="C45">
+        <v>38.702026438267701</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>259</v>
+      </c>
+      <c r="B46">
+        <v>-75.563800000000001</v>
+      </c>
+      <c r="C46">
+        <v>39.838700000000003</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>261</v>
+      </c>
+      <c r="B47">
+        <v>-68.211070000000007</v>
+      </c>
+      <c r="C47">
+        <v>44.349651999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>274</v>
+      </c>
+      <c r="B48">
+        <v>-79.911533000000006</v>
+      </c>
+      <c r="C48">
+        <v>43.468915000000003</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>278</v>
+      </c>
+      <c r="B49">
+        <v>-64.167955000000006</v>
+      </c>
+      <c r="C49">
+        <v>44.992969000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>282</v>
+      </c>
+      <c r="B50">
+        <v>-66.050550000000001</v>
+      </c>
+      <c r="C50">
+        <v>45.300289999999997</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>286</v>
+      </c>
+      <c r="B51">
+        <v>-64.476939999999999</v>
+      </c>
+      <c r="C51">
+        <v>45.93694</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added R doc for making new data table, updated/added data tables
</commit_message>
<xml_diff>
--- a/data/01_pd-samples/26_01_15_pd_samples-edited.xlsx
+++ b/data/01_pd-samples/26_01_15_pd_samples-edited.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caprinapugliese/Documents/School/Uconn/2024-26_Grad_School/Dagilis-lab/WNS-project/data/01_pd-samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4118014C-9462-8646-B4A1-605D4A34AC68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6516167-3414-AE4D-B5E4-490DA48775C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27740" windowHeight="17500" activeTab="3" xr2:uid="{D99E271A-162C-F24C-8D0E-BBA6ED327C07}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27740" windowHeight="17500" activeTab="1" xr2:uid="{D99E271A-162C-F24C-8D0E-BBA6ED327C07}"/>
   </bookViews>
   <sheets>
     <sheet name="25_10-16_pd_samples-edited" sheetId="1" r:id="rId1"/>
@@ -6769,8 +6769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BD2066C-9D82-5444-90C3-5EB5DCC8324A}">
   <dimension ref="A1:X52"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10327,8 +10327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76291800-C65C-8C4F-9D97-BB7E20AAC35D}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
made pca plots for ALL pd samples
</commit_message>
<xml_diff>
--- a/data/01_pd-samples/26_01_15_pd_samples-edited.xlsx
+++ b/data/01_pd-samples/26_01_15_pd_samples-edited.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caprinapugliese/Documents/School/Uconn/2024-26_Grad_School/Dagilis-lab/WNS-project/data/01_pd-samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07FA168E-D86B-FB40-9895-6533A86FBA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0F57A4-115F-2845-A58C-02BA24A6F338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27740" windowHeight="17500" activeTab="5" xr2:uid="{D99E271A-162C-F24C-8D0E-BBA6ED327C07}"/>
+    <workbookView xWindow="4460" yWindow="1300" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{D99E271A-162C-F24C-8D0E-BBA6ED327C07}"/>
   </bookViews>
   <sheets>
     <sheet name="25_10-16_pd_samples-edited" sheetId="1" r:id="rId1"/>
-    <sheet name="25_10-16_pd_samples-edited (2)" sheetId="6" r:id="rId2"/>
+    <sheet name="pd_only" sheetId="9" r:id="rId2"/>
     <sheet name="pd_northamer_only" sheetId="2" r:id="rId3"/>
     <sheet name="NoA_Pd_coords" sheetId="3" r:id="rId4"/>
     <sheet name="no washington" sheetId="5" r:id="rId5"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3583" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3456" uniqueCount="426">
   <si>
     <t>sample_id</t>
   </si>
@@ -1881,7 +1881,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1923,7 +1923,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="42" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1934,7 +1934,6 @@
     </xf>
     <xf numFmtId="14" fontId="22" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2039,8 +2038,8 @@
     <tableColumn id="1" xr3:uid="{30EFF156-3D30-484A-8AD7-EA85D1CE06B4}" name="sample_id"/>
     <tableColumn id="2" xr3:uid="{A57D6E87-53D9-9040-A419-D8F9EB108C4C}" name="individuals"/>
     <tableColumn id="24" xr3:uid="{3B742AA1-E6CD-E149-8D76-9BF45791B0CA}" name="names"/>
-    <tableColumn id="23" xr3:uid="{696A16A2-3458-2749-BBFE-412CD7189CD5}" name="sra_number" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{2A54557F-8AB7-7F43-877C-FD7C0EA8D35A}" name="sra" dataDxfId="4"/>
+    <tableColumn id="23" xr3:uid="{696A16A2-3458-2749-BBFE-412CD7189CD5}" name="sra_number" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{2A54557F-8AB7-7F43-877C-FD7C0EA8D35A}" name="sra" dataDxfId="7"/>
     <tableColumn id="4" xr3:uid="{BDE76617-CD6A-DC47-AB84-5ECFBE4656EA}" name="platform"/>
     <tableColumn id="5" xr3:uid="{8E9655EC-1F75-A54B-A3E9-4D24F04D79E1}" name="library"/>
     <tableColumn id="18" xr3:uid="{E29A7C29-3FAA-594A-8F1C-A5BD70E3E221}" name="year"/>
@@ -2058,7 +2057,7 @@
     <tableColumn id="19" xr3:uid="{180BBF41-7859-AE4D-9DB9-B4899CCD75FC}" name="sra_project"/>
     <tableColumn id="15" xr3:uid="{C8CDD26B-E025-644D-850C-479D08FC207A}" name="provider"/>
     <tableColumn id="21" xr3:uid="{1F073B69-2EEB-4F4E-A4F7-CF5A32E0C613}" name="strain"/>
-    <tableColumn id="16" xr3:uid="{5A8723C2-EA7F-804A-A08F-C0FD996227E9}" name="citation" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{5A8723C2-EA7F-804A-A08F-C0FD996227E9}" name="citation" dataDxfId="6"/>
     <tableColumn id="17" xr3:uid="{804E7016-075C-2E4B-B8E7-6333BEF7B9EA}" name="notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2066,42 +2065,36 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{26542971-EE17-0644-8379-1EE9FBEBE87D}" name="Table14" displayName="Table14" ref="A1:X75" totalsRowShown="0">
-  <autoFilter ref="A1:X75" xr:uid="{90C14361-2949-B74A-BFF6-1CEFD0790204}">
-    <filterColumn colId="11">
-      <filters>
-        <filter val="N_America"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X75">
-    <sortCondition ref="B1:B75"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{18C33721-6494-9A49-9427-66EBEE919E8D}" name="Table14" displayName="Table14" ref="A1:X68" totalsRowShown="0">
+  <autoFilter ref="A1:X68" xr:uid="{90C14361-2949-B74A-BFF6-1CEFD0790204}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X68">
+    <sortCondition ref="B1:B68"/>
   </sortState>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{45058D78-BF6A-A44D-9AC8-B433A38DF5CB}" name="sample_id"/>
-    <tableColumn id="2" xr3:uid="{259CCAF3-AA94-A747-99FA-1B53D83AAE07}" name="individuals"/>
-    <tableColumn id="24" xr3:uid="{EE42D89C-6934-6C4D-8707-D025E390DCE0}" name="names"/>
-    <tableColumn id="23" xr3:uid="{2DFC13FD-2415-2A45-99AF-99C9693E4428}" name="sra_number" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{D40F3198-9777-F543-82CC-CC2964B91BEF}" name="sra" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{C87E2A9E-9056-D04C-A8C3-4A45957E45B5}" name="platform"/>
-    <tableColumn id="5" xr3:uid="{E4BB5BDA-F443-A246-B33A-D6F0381250AF}" name="library"/>
-    <tableColumn id="18" xr3:uid="{230019CA-D27E-6649-A406-E394C3D3DF81}" name="year"/>
-    <tableColumn id="6" xr3:uid="{9D9D0998-75AE-9142-A288-9E82E844A77F}" name="collection_date"/>
-    <tableColumn id="7" xr3:uid="{C25FB2FF-C1EC-BD44-B03A-7595893AC486}" name="instrument"/>
-    <tableColumn id="8" xr3:uid="{C069DA0B-99E6-0D4D-917B-FFDC6036CAF5}" name="strat"/>
-    <tableColumn id="9" xr3:uid="{9CE122A7-60D6-104D-87CE-D7A08B416515}" name="continent"/>
-    <tableColumn id="10" xr3:uid="{BEBD32C3-7FD6-964B-94B4-AA52332F2387}" name="country"/>
-    <tableColumn id="11" xr3:uid="{533800A1-A008-A944-9A2D-9C5153CF538D}" name="state"/>
-    <tableColumn id="12" xr3:uid="{DCA7C53B-067C-FA44-980A-1B003276BEB9}" name="location"/>
-    <tableColumn id="25" xr3:uid="{8E1CC910-336F-854D-BCED-154601593C72}" name="isolate_location"/>
-    <tableColumn id="13" xr3:uid="{7243FDD1-8223-2049-AACB-950F09A8DB1E}" name="lat"/>
-    <tableColumn id="14" xr3:uid="{8600DBBA-573A-DA48-B628-84F365894F7A}" name="long"/>
-    <tableColumn id="20" xr3:uid="{9E1C8029-B54E-FD40-963E-CC17DB276AEF}" name="bioproject"/>
-    <tableColumn id="19" xr3:uid="{0943EC97-A9B2-1948-A4CB-9EEEF088171C}" name="sra_project"/>
-    <tableColumn id="15" xr3:uid="{6CB29598-9800-154C-B5D1-0998BF8349A2}" name="provider"/>
-    <tableColumn id="21" xr3:uid="{A440A3DE-0AF5-8344-94CF-4C905D3A2867}" name="strain"/>
-    <tableColumn id="16" xr3:uid="{012E999B-7CF7-7847-8716-9E55EB6964D9}" name="citation" dataDxfId="0"/>
-    <tableColumn id="17" xr3:uid="{31C25CAC-5465-F740-9E7F-57DD054A5E38}" name="notes"/>
+    <tableColumn id="1" xr3:uid="{B94284E2-80D9-FD40-B6D3-31E24510FDA8}" name="sample_id"/>
+    <tableColumn id="2" xr3:uid="{49E2AAE4-EF8C-254F-A868-67210D9E479C}" name="individuals"/>
+    <tableColumn id="24" xr3:uid="{DB5FBE05-1902-4945-A834-7AB497F9D24A}" name="names"/>
+    <tableColumn id="23" xr3:uid="{5BBAC386-EE03-5341-8256-FCC0EA039DDC}" name="sra_number" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{44BC2290-DD2A-2C47-B9D0-41700864ED16}" name="sra" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{A32FD781-B2BC-F545-84E8-C1E3D8B4B972}" name="platform"/>
+    <tableColumn id="5" xr3:uid="{34F4B79A-B462-AA4D-916E-1559C61C3C92}" name="library"/>
+    <tableColumn id="18" xr3:uid="{786EDAD5-AFEC-A645-83EE-752E1079232A}" name="year"/>
+    <tableColumn id="6" xr3:uid="{FFCA6E2A-A7A1-D34C-8AD7-7F50EF7C1EF8}" name="collection_date"/>
+    <tableColumn id="7" xr3:uid="{C2D9F4B2-D77A-8544-B957-4D7D7EEF3125}" name="instrument"/>
+    <tableColumn id="8" xr3:uid="{9B2495C9-CB8F-2C42-9EC9-576D7A84F239}" name="strat"/>
+    <tableColumn id="9" xr3:uid="{28A4AFAC-0441-4E44-84EB-8CA5D9D0FAB1}" name="continent"/>
+    <tableColumn id="10" xr3:uid="{DE39B635-1AD0-AC4F-A5F9-9B71EA841760}" name="country"/>
+    <tableColumn id="11" xr3:uid="{34A911D2-3D76-DD42-92EB-5431D8D36D00}" name="state"/>
+    <tableColumn id="12" xr3:uid="{7F29B3F8-E375-0A40-AA2C-ED13839F3068}" name="location"/>
+    <tableColumn id="25" xr3:uid="{19200440-D88A-8040-9F15-46BBC19C72C5}" name="isolate_location"/>
+    <tableColumn id="13" xr3:uid="{388A7953-67AC-1146-8EB4-30DA74019984}" name="lat"/>
+    <tableColumn id="14" xr3:uid="{191C8100-8FA0-784A-B3AA-6D02D9D2C9ED}" name="long"/>
+    <tableColumn id="20" xr3:uid="{6DA3CD2D-ECF2-774F-86B4-257E0527D655}" name="bioproject"/>
+    <tableColumn id="19" xr3:uid="{962EE038-25A2-C649-A4CD-E544474BB2C7}" name="sra_project"/>
+    <tableColumn id="15" xr3:uid="{99D4037E-5084-F447-895C-D7A50CA77A52}" name="provider"/>
+    <tableColumn id="21" xr3:uid="{B29A4A21-C30E-6247-ACCF-4B943FDBC4CA}" name="strain"/>
+    <tableColumn id="16" xr3:uid="{47CC5497-CBA3-AF4A-AA11-8275AFC1B401}" name="citation" dataDxfId="0"/>
+    <tableColumn id="17" xr3:uid="{7A8AC5A7-55F5-8443-A572-9EDB06FCC139}" name="notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2117,8 +2110,8 @@
     <tableColumn id="1" xr3:uid="{684E08F5-2427-9C44-9268-566A0648100F}" name="sample_id"/>
     <tableColumn id="2" xr3:uid="{9E5085F7-1454-BD45-B35E-CA86CE65B6C4}" name="individuals"/>
     <tableColumn id="24" xr3:uid="{A45F8857-AEC6-B347-9C32-F2C545BF257B}" name="names"/>
-    <tableColumn id="23" xr3:uid="{25542BD2-CC8B-3E45-AB7B-AFF483FB49BB}" name="sra_number" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{244999BB-BE64-8140-91F6-D731D74E5E80}" name="sra" dataDxfId="7"/>
+    <tableColumn id="23" xr3:uid="{25542BD2-CC8B-3E45-AB7B-AFF483FB49BB}" name="sra_number" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{244999BB-BE64-8140-91F6-D731D74E5E80}" name="sra" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{AE1F9C30-7582-DB45-8E54-033532F79C18}" name="platform"/>
     <tableColumn id="5" xr3:uid="{BC854B37-FE43-7D4A-AFF2-D0247CFE9CE1}" name="library"/>
     <tableColumn id="18" xr3:uid="{6F509B67-3012-8548-A7A1-D33349479471}" name="year"/>
@@ -2136,7 +2129,7 @@
     <tableColumn id="19" xr3:uid="{4AEEEA9E-4D1C-4E4F-9B8C-7ED4DC180965}" name="sra_project"/>
     <tableColumn id="15" xr3:uid="{FAF37CB6-DD9E-A041-AE6A-7BFF50540EFF}" name="provider"/>
     <tableColumn id="21" xr3:uid="{2DFA1BDD-9C74-B942-803C-0BBF64B6B912}" name="strain"/>
-    <tableColumn id="16" xr3:uid="{63C77C5B-6E69-F146-897C-ADF38B1DB69C}" name="citation" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{63C77C5B-6E69-F146-897C-ADF38B1DB69C}" name="citation" dataDxfId="3"/>
     <tableColumn id="17" xr3:uid="{4B2A6BBE-1B07-6F48-861C-06AF0F613B24}" name="notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2462,8 +2455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E4D9535-1238-AB48-B467-419735026371}">
   <dimension ref="A1:X75"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2473,11 +2466,11 @@
     <col min="3" max="3" width="41.6640625" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" style="5" customWidth="1"/>
     <col min="5" max="5" width="15.5" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="4" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="4" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" customWidth="1"/>
     <col min="12" max="12" width="11.33203125" customWidth="1"/>
     <col min="13" max="13" width="14.1640625" customWidth="1"/>
     <col min="14" max="14" width="25.6640625" customWidth="1"/>
@@ -6920,25 +6913,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{623EA130-3154-2A42-B760-E9CDE28657EF}">
-  <dimension ref="A1:X75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81932B95-B62D-A841-B6E7-B8639D22EAB5}">
+  <dimension ref="A1:X68"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:X75"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="41.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" style="5" customWidth="1"/>
     <col min="5" max="5" width="15.5" style="4" customWidth="1"/>
-    <col min="6" max="6" width="16.1640625" customWidth="1"/>
-    <col min="7" max="7" width="19.1640625" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="22.33203125" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" customWidth="1"/>
     <col min="12" max="12" width="11.33203125" customWidth="1"/>
     <col min="13" max="13" width="14.1640625" customWidth="1"/>
     <col min="14" max="14" width="25.6640625" customWidth="1"/>
@@ -7086,7 +7079,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -7151,7 +7144,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -7216,7 +7209,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -7281,7 +7274,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="34" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -7995,7 +7988,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="18" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>85</v>
       </c>
@@ -8573,39 +8566,39 @@
         <v>387</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>126</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>126</v>
+        <v>154</v>
+      </c>
+      <c r="B28" t="s">
+        <v>155</v>
+      </c>
+      <c r="C28" t="s">
+        <v>154</v>
       </c>
       <c r="D28" s="5">
-        <v>1955487</v>
+        <v>29259</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="F28" t="s">
         <v>51</v>
       </c>
       <c r="G28" t="s">
-        <v>129</v>
+        <v>157</v>
       </c>
       <c r="H28">
-        <v>2008</v>
-      </c>
-      <c r="I28">
-        <v>2008</v>
+        <v>2009</v>
+      </c>
+      <c r="I28" s="1">
+        <v>40073</v>
       </c>
       <c r="J28" t="s">
-        <v>130</v>
+        <v>158</v>
       </c>
       <c r="K28" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="L28" t="s">
         <v>20</v>
@@ -8614,69 +8607,69 @@
         <v>298</v>
       </c>
       <c r="N28" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="O28" t="s">
-        <v>305</v>
-      </c>
-      <c r="P28" t="s">
-        <v>394</v>
+        <v>328</v>
       </c>
       <c r="Q28">
-        <v>43.835385505600499</v>
+        <v>41.844515371877698</v>
       </c>
       <c r="R28">
-        <v>-92.283091749633499</v>
+        <v>-74.098548155198898</v>
       </c>
       <c r="S28" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="T28" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="U28" t="s">
-        <v>378</v>
-      </c>
-      <c r="V28" s="7" t="s">
-        <v>397</v>
-      </c>
-      <c r="W28" s="6" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" ht="51" hidden="1" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="V28" t="s">
+        <v>384</v>
+      </c>
+      <c r="W28" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="X28" s="2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>131</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>131</v>
+        <v>154</v>
+      </c>
+      <c r="B29" t="s">
+        <v>159</v>
+      </c>
+      <c r="C29" t="s">
+        <v>154</v>
       </c>
       <c r="D29" s="5">
-        <v>1955239</v>
+        <v>29260</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>133</v>
+        <v>160</v>
       </c>
       <c r="F29" t="s">
         <v>51</v>
       </c>
       <c r="G29" t="s">
-        <v>134</v>
+        <v>161</v>
       </c>
       <c r="H29">
-        <v>1960</v>
-      </c>
-      <c r="I29">
-        <v>1960</v>
+        <v>2009</v>
+      </c>
+      <c r="I29" s="1">
+        <v>40073</v>
       </c>
       <c r="J29" t="s">
-        <v>117</v>
+        <v>158</v>
       </c>
       <c r="K29" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="L29" t="s">
         <v>20</v>
@@ -8685,69 +8678,66 @@
         <v>298</v>
       </c>
       <c r="N29" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="O29" t="s">
-        <v>305</v>
-      </c>
-      <c r="P29" t="s">
-        <v>392</v>
+        <v>328</v>
       </c>
       <c r="Q29">
-        <v>45.876656556660201</v>
+        <v>41.844515371877698</v>
       </c>
       <c r="R29">
-        <v>-89.628365849641099</v>
+        <v>-74.098548155198898</v>
       </c>
       <c r="S29" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="T29" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="U29" t="s">
-        <v>378</v>
-      </c>
-      <c r="V29" s="7" t="s">
-        <v>390</v>
-      </c>
-      <c r="W29" s="6" t="s">
-        <v>386</v>
-      </c>
-      <c r="X29" s="2" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="V29" t="s">
+        <v>384</v>
+      </c>
+      <c r="W29" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="X29" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>135</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>135</v>
+        <v>154</v>
+      </c>
+      <c r="B30" t="s">
+        <v>162</v>
+      </c>
+      <c r="C30" t="s">
+        <v>154</v>
       </c>
       <c r="D30" s="5">
-        <v>1955482</v>
+        <v>31784</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>137</v>
+        <v>163</v>
       </c>
       <c r="F30" t="s">
         <v>51</v>
       </c>
       <c r="G30" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="H30">
-        <v>2002</v>
-      </c>
-      <c r="I30">
-        <v>2002</v>
+        <v>2009</v>
+      </c>
+      <c r="I30" s="1">
+        <v>40073</v>
       </c>
       <c r="J30" t="s">
-        <v>117</v>
+        <v>158</v>
       </c>
       <c r="K30" t="s">
         <v>43</v>
@@ -8756,69 +8746,69 @@
         <v>20</v>
       </c>
       <c r="M30" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="N30" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="O30" t="s">
-        <v>305</v>
-      </c>
-      <c r="P30" t="s">
-        <v>391</v>
+        <v>328</v>
       </c>
       <c r="Q30">
-        <v>53.933300000000003</v>
+        <v>41.844515371877698</v>
       </c>
       <c r="R30">
-        <v>-116.5765</v>
+        <v>-74.098548155198898</v>
       </c>
       <c r="S30" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="T30" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="U30" t="s">
-        <v>378</v>
-      </c>
-      <c r="V30" s="7" t="s">
-        <v>389</v>
-      </c>
-      <c r="W30" s="6" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="V30" t="s">
+        <v>384</v>
+      </c>
+      <c r="W30" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="X30" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>139</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>139</v>
+        <v>154</v>
+      </c>
+      <c r="B31" t="s">
+        <v>165</v>
+      </c>
+      <c r="C31" t="s">
+        <v>154</v>
       </c>
       <c r="D31" s="5">
-        <v>1955483</v>
+        <v>107675</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="F31" t="s">
         <v>51</v>
       </c>
       <c r="G31" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="H31">
-        <v>2008</v>
-      </c>
-      <c r="I31">
-        <v>2008</v>
+        <v>2009</v>
+      </c>
+      <c r="I31" s="1">
+        <v>40073</v>
       </c>
       <c r="J31" t="s">
-        <v>117</v>
+        <v>158</v>
       </c>
       <c r="K31" t="s">
         <v>43</v>
@@ -8830,211 +8820,181 @@
         <v>298</v>
       </c>
       <c r="N31" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="O31" t="s">
-        <v>305</v>
-      </c>
-      <c r="P31" t="s">
-        <v>394</v>
+        <v>328</v>
       </c>
       <c r="Q31">
-        <v>42.871989999999997</v>
+        <v>41.844515371877698</v>
       </c>
       <c r="R31">
-        <v>-73.226607000000001</v>
+        <v>-74.098548155198898</v>
       </c>
       <c r="S31" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="T31" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="U31" t="s">
-        <v>378</v>
-      </c>
-      <c r="V31" s="7" t="s">
-        <v>393</v>
-      </c>
-      <c r="W31" s="6" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="V31" t="s">
+        <v>384</v>
+      </c>
+      <c r="W31" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="X31" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>143</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>143</v>
+        <v>168</v>
+      </c>
+      <c r="B32" t="s">
+        <v>169</v>
+      </c>
+      <c r="C32" t="s">
+        <v>168</v>
       </c>
       <c r="D32" s="5">
-        <v>1955484</v>
+        <v>6011467</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>145</v>
+        <v>170</v>
       </c>
       <c r="F32" t="s">
         <v>51</v>
       </c>
       <c r="G32" t="s">
-        <v>146</v>
+        <v>171</v>
       </c>
       <c r="H32">
-        <v>2008</v>
-      </c>
-      <c r="I32">
-        <v>2008</v>
+        <v>2009</v>
+      </c>
+      <c r="I32" s="1">
+        <v>39879</v>
       </c>
       <c r="J32" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="K32" t="s">
         <v>43</v>
       </c>
-      <c r="L32" t="s">
-        <v>20</v>
+      <c r="L32" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="M32" t="s">
-        <v>298</v>
+        <v>323</v>
       </c>
       <c r="N32" t="s">
-        <v>299</v>
+        <v>324</v>
       </c>
       <c r="O32" t="s">
         <v>305</v>
       </c>
-      <c r="P32" t="s">
-        <v>394</v>
-      </c>
       <c r="Q32">
-        <v>41.844515371877698</v>
+        <v>50.788476564399403</v>
       </c>
       <c r="R32">
-        <v>-74.098548155198898</v>
-      </c>
-      <c r="S32" t="s">
-        <v>379</v>
-      </c>
-      <c r="T32" t="s">
-        <v>380</v>
-      </c>
-      <c r="U32" t="s">
-        <v>378</v>
-      </c>
-      <c r="V32" s="7" t="s">
-        <v>396</v>
-      </c>
-      <c r="W32" s="6" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="33" spans="1:24" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>10.740499703414899</v>
+      </c>
+      <c r="X32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>147</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>147</v>
+        <v>171</v>
+      </c>
+      <c r="B33" t="s">
+        <v>172</v>
+      </c>
+      <c r="C33" t="s">
+        <v>171</v>
       </c>
       <c r="D33" s="5">
-        <v>1955485</v>
+        <v>6011468</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>149</v>
+        <v>173</v>
       </c>
       <c r="F33" t="s">
         <v>51</v>
       </c>
       <c r="G33" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="H33">
-        <v>2008</v>
-      </c>
-      <c r="I33">
-        <v>2008</v>
+        <v>2009</v>
+      </c>
+      <c r="I33" s="1">
+        <v>39904</v>
       </c>
       <c r="J33" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="K33" t="s">
         <v>43</v>
       </c>
-      <c r="L33" t="s">
-        <v>20</v>
+      <c r="L33" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="M33" t="s">
-        <v>298</v>
+        <v>336</v>
       </c>
       <c r="N33" t="s">
-        <v>302</v>
+        <v>338</v>
       </c>
       <c r="O33" t="s">
         <v>305</v>
       </c>
-      <c r="P33" s="2" t="s">
-        <v>407</v>
-      </c>
       <c r="Q33">
-        <v>45.876656556660201</v>
+        <v>47.083329999999997</v>
       </c>
       <c r="R33">
-        <v>-89.628365849641099</v>
-      </c>
-      <c r="S33" t="s">
-        <v>379</v>
-      </c>
-      <c r="T33" t="s">
-        <v>380</v>
-      </c>
-      <c r="U33" t="s">
-        <v>378</v>
-      </c>
-      <c r="V33" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="W33" s="6" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="X33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>126</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>126</v>
+        <v>174</v>
+      </c>
+      <c r="B34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C34" t="s">
+        <v>174</v>
       </c>
       <c r="D34" s="5">
-        <v>1955486</v>
+        <v>6011469</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>152</v>
+        <v>176</v>
       </c>
       <c r="F34" t="s">
         <v>51</v>
       </c>
       <c r="G34" t="s">
-        <v>153</v>
+        <v>177</v>
       </c>
       <c r="H34">
-        <v>2008</v>
-      </c>
-      <c r="I34">
-        <v>2008</v>
+        <v>2009</v>
+      </c>
+      <c r="I34" s="1">
+        <v>39897</v>
       </c>
       <c r="J34" t="s">
-        <v>18</v>
+        <v>130</v>
       </c>
       <c r="K34" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="L34" t="s">
         <v>20</v>
@@ -9043,69 +9003,51 @@
         <v>298</v>
       </c>
       <c r="N34" t="s">
-        <v>301</v>
+        <v>339</v>
       </c>
       <c r="O34" t="s">
-        <v>305</v>
-      </c>
-      <c r="P34" t="s">
-        <v>394</v>
+        <v>340</v>
       </c>
       <c r="Q34">
-        <v>43.835385505600499</v>
+        <v>40.888610999999997</v>
       </c>
       <c r="R34">
-        <v>-92.283091749633499</v>
-      </c>
-      <c r="S34" t="s">
-        <v>379</v>
-      </c>
-      <c r="T34" t="s">
-        <v>380</v>
-      </c>
-      <c r="U34" t="s">
-        <v>378</v>
-      </c>
-      <c r="V34" s="7" t="s">
-        <v>397</v>
-      </c>
-      <c r="W34" s="6" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="35" spans="1:24" ht="34" hidden="1" x14ac:dyDescent="0.2">
+        <v>-77.386111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="B35" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
       <c r="C35" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="D35" s="5">
-        <v>29259</v>
+        <v>6011470</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
       <c r="F35" t="s">
         <v>51</v>
       </c>
       <c r="G35" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="H35">
         <v>2009</v>
       </c>
       <c r="I35" s="1">
-        <v>40073</v>
+        <v>39990</v>
       </c>
       <c r="J35" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="K35" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="L35" t="s">
         <v>20</v>
@@ -9114,69 +9056,51 @@
         <v>298</v>
       </c>
       <c r="N35" t="s">
-        <v>299</v>
+        <v>341</v>
       </c>
       <c r="O35" t="s">
-        <v>328</v>
+        <v>342</v>
       </c>
       <c r="Q35">
-        <v>41.844515371877698</v>
+        <v>40.877385651285401</v>
       </c>
       <c r="R35">
-        <v>-74.098548155198898</v>
-      </c>
-      <c r="S35" t="s">
-        <v>381</v>
-      </c>
-      <c r="T35" t="s">
-        <v>382</v>
-      </c>
-      <c r="U35" t="s">
-        <v>330</v>
-      </c>
-      <c r="V35" t="s">
-        <v>384</v>
-      </c>
-      <c r="W35" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="X35" s="2" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="36" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+        <v>-74.968855407371393</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
       <c r="B36" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
       <c r="C36" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
       <c r="D36" s="5">
-        <v>29260</v>
+        <v>6011471</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>160</v>
+        <v>182</v>
       </c>
       <c r="F36" t="s">
         <v>51</v>
       </c>
       <c r="G36" t="s">
-        <v>161</v>
+        <v>183</v>
       </c>
       <c r="H36">
         <v>2009</v>
       </c>
       <c r="I36" s="1">
-        <v>40073</v>
+        <v>39843</v>
       </c>
       <c r="J36" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="K36" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="L36" t="s">
         <v>20</v>
@@ -9185,66 +9109,48 @@
         <v>298</v>
       </c>
       <c r="N36" t="s">
-        <v>299</v>
+        <v>343</v>
       </c>
       <c r="O36" t="s">
-        <v>328</v>
+        <v>344</v>
       </c>
       <c r="Q36">
-        <v>41.844515371877698</v>
+        <v>38.664935999999997</v>
       </c>
       <c r="R36">
-        <v>-74.098548155198898</v>
-      </c>
-      <c r="S36" t="s">
-        <v>381</v>
-      </c>
-      <c r="T36" t="s">
-        <v>382</v>
-      </c>
-      <c r="U36" t="s">
-        <v>330</v>
-      </c>
-      <c r="V36" t="s">
-        <v>384</v>
-      </c>
-      <c r="W36" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="X36" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="37" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+        <v>-79.430160999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>154</v>
+        <v>183</v>
       </c>
       <c r="B37" t="s">
-        <v>162</v>
+        <v>184</v>
       </c>
       <c r="C37" t="s">
-        <v>154</v>
+        <v>183</v>
       </c>
       <c r="D37" s="5">
-        <v>31784</v>
+        <v>6011472</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>163</v>
+        <v>185</v>
       </c>
       <c r="F37" t="s">
         <v>51</v>
       </c>
       <c r="G37" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="H37">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="I37" s="1">
-        <v>40073</v>
+        <v>40248</v>
       </c>
       <c r="J37" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="K37" t="s">
         <v>43</v>
@@ -9253,69 +9159,51 @@
         <v>20</v>
       </c>
       <c r="M37" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="N37" t="s">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="O37" t="s">
-        <v>328</v>
+        <v>345</v>
       </c>
       <c r="Q37">
-        <v>41.844515371877698</v>
+        <v>48.174337000000001</v>
       </c>
       <c r="R37">
-        <v>-74.098548155198898</v>
-      </c>
-      <c r="S37" t="s">
-        <v>381</v>
-      </c>
-      <c r="T37" t="s">
-        <v>382</v>
-      </c>
-      <c r="U37" t="s">
-        <v>330</v>
-      </c>
-      <c r="V37" t="s">
-        <v>384</v>
-      </c>
-      <c r="W37" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="X37" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="38" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+        <v>-80.100126000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>154</v>
+        <v>186</v>
       </c>
       <c r="B38" t="s">
-        <v>165</v>
+        <v>187</v>
       </c>
       <c r="C38" t="s">
-        <v>154</v>
+        <v>186</v>
       </c>
       <c r="D38" s="5">
-        <v>107675</v>
+        <v>6011473</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>166</v>
+        <v>188</v>
       </c>
       <c r="F38" t="s">
         <v>51</v>
       </c>
       <c r="G38" t="s">
-        <v>167</v>
+        <v>189</v>
       </c>
       <c r="H38">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="I38" s="1">
-        <v>40073</v>
+        <v>40242</v>
       </c>
       <c r="J38" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="K38" t="s">
         <v>43</v>
@@ -9327,119 +9215,98 @@
         <v>298</v>
       </c>
       <c r="N38" t="s">
-        <v>299</v>
+        <v>354</v>
       </c>
       <c r="O38" t="s">
-        <v>328</v>
+        <v>366</v>
       </c>
       <c r="Q38">
-        <v>41.844515371877698</v>
+        <v>36.555458999999999</v>
       </c>
       <c r="R38">
-        <v>-74.098548155198898</v>
-      </c>
-      <c r="S38" t="s">
-        <v>381</v>
-      </c>
-      <c r="T38" t="s">
-        <v>382</v>
-      </c>
-      <c r="U38" t="s">
-        <v>330</v>
-      </c>
-      <c r="V38" t="s">
-        <v>384</v>
-      </c>
-      <c r="W38" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="X38" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="39" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+        <v>-87.304068999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>168</v>
+        <v>189</v>
       </c>
       <c r="B39" t="s">
-        <v>169</v>
+        <v>190</v>
       </c>
       <c r="C39" t="s">
-        <v>168</v>
+        <v>189</v>
       </c>
       <c r="D39" s="5">
-        <v>6011467</v>
+        <v>6011474</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
       <c r="F39" t="s">
         <v>51</v>
       </c>
       <c r="G39" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="H39">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="I39" s="1">
-        <v>39879</v>
+        <v>39525</v>
       </c>
       <c r="J39" t="s">
-        <v>130</v>
+        <v>193</v>
       </c>
       <c r="K39" t="s">
         <v>43</v>
       </c>
-      <c r="L39" s="10" t="s">
-        <v>25</v>
+      <c r="L39" t="s">
+        <v>20</v>
       </c>
       <c r="M39" t="s">
-        <v>323</v>
+        <v>298</v>
       </c>
       <c r="N39" t="s">
-        <v>324</v>
+        <v>304</v>
       </c>
       <c r="O39" t="s">
-        <v>305</v>
+        <v>360</v>
       </c>
       <c r="Q39">
-        <v>50.788476564399403</v>
+        <v>42.871989999999997</v>
       </c>
       <c r="R39">
-        <v>10.740499703414899</v>
-      </c>
-      <c r="X39" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="40" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+        <v>-73.226607000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="B40" t="s">
-        <v>172</v>
+        <v>194</v>
       </c>
       <c r="C40" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="D40" s="5">
-        <v>6011468</v>
+        <v>6011475</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>173</v>
+        <v>195</v>
       </c>
       <c r="F40" t="s">
         <v>51</v>
       </c>
       <c r="G40" t="s">
-        <v>174</v>
+        <v>196</v>
       </c>
       <c r="H40">
         <v>2009</v>
       </c>
       <c r="I40" s="1">
-        <v>39904</v>
+        <v>39840</v>
       </c>
       <c r="J40" t="s">
         <v>130</v>
@@ -9447,55 +9314,52 @@
       <c r="K40" t="s">
         <v>43</v>
       </c>
-      <c r="L40" s="10" t="s">
-        <v>25</v>
+      <c r="L40" t="s">
+        <v>20</v>
       </c>
       <c r="M40" t="s">
-        <v>336</v>
+        <v>298</v>
       </c>
       <c r="N40" t="s">
-        <v>338</v>
+        <v>349</v>
       </c>
       <c r="O40" t="s">
-        <v>305</v>
+        <v>350</v>
       </c>
       <c r="Q40">
-        <v>47.083329999999997</v>
+        <v>41.745700999999997</v>
       </c>
       <c r="R40">
-        <v>8</v>
-      </c>
-      <c r="X40" t="s">
-        <v>26</v>
+        <v>-73.158473999999998</v>
       </c>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>174</v>
+        <v>196</v>
       </c>
       <c r="B41" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="C41" t="s">
-        <v>174</v>
+        <v>196</v>
       </c>
       <c r="D41" s="5">
-        <v>6011469</v>
+        <v>6011476</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>176</v>
+        <v>198</v>
       </c>
       <c r="F41" t="s">
         <v>51</v>
       </c>
       <c r="G41" t="s">
-        <v>177</v>
+        <v>199</v>
       </c>
       <c r="H41">
         <v>2009</v>
       </c>
       <c r="I41" s="1">
-        <v>39897</v>
+        <v>39875</v>
       </c>
       <c r="J41" t="s">
         <v>130</v>
@@ -9510,45 +9374,45 @@
         <v>298</v>
       </c>
       <c r="N41" t="s">
-        <v>339</v>
+        <v>351</v>
       </c>
       <c r="O41" t="s">
-        <v>340</v>
+        <v>352</v>
       </c>
       <c r="Q41">
-        <v>40.888610999999997</v>
+        <v>37.322156999999997</v>
       </c>
       <c r="R41">
-        <v>-77.386111</v>
+        <v>-80.756189000000006</v>
       </c>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>177</v>
+        <v>199</v>
       </c>
       <c r="B42" t="s">
-        <v>178</v>
+        <v>200</v>
       </c>
       <c r="C42" t="s">
-        <v>177</v>
+        <v>199</v>
       </c>
       <c r="D42" s="5">
-        <v>6011470</v>
+        <v>6011477</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>179</v>
+        <v>201</v>
       </c>
       <c r="F42" t="s">
         <v>51</v>
       </c>
       <c r="G42" t="s">
-        <v>180</v>
+        <v>202</v>
       </c>
       <c r="H42">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="I42" s="1">
-        <v>39990</v>
+        <v>39528</v>
       </c>
       <c r="J42" t="s">
         <v>130</v>
@@ -9563,51 +9427,51 @@
         <v>298</v>
       </c>
       <c r="N42" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
       <c r="O42" t="s">
-        <v>342</v>
+        <v>361</v>
       </c>
       <c r="Q42">
-        <v>40.877385651285401</v>
+        <v>42.592351000000001</v>
       </c>
       <c r="R42">
-        <v>-74.968855407371393</v>
-      </c>
-    </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
+        <v>-73.226241999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>180</v>
+        <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>181</v>
+        <v>203</v>
       </c>
       <c r="C43" t="s">
-        <v>180</v>
+        <v>41</v>
       </c>
       <c r="D43" s="5">
-        <v>6011471</v>
+        <v>3545532</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>182</v>
+        <v>204</v>
       </c>
       <c r="F43" t="s">
         <v>51</v>
       </c>
       <c r="G43" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="H43">
-        <v>2009</v>
-      </c>
-      <c r="I43" s="1">
-        <v>39843</v>
+        <v>2015</v>
+      </c>
+      <c r="I43">
+        <v>2015</v>
       </c>
       <c r="J43" t="s">
-        <v>130</v>
+        <v>18</v>
       </c>
       <c r="K43" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="L43" t="s">
         <v>20</v>
@@ -9616,98 +9480,116 @@
         <v>298</v>
       </c>
       <c r="N43" t="s">
-        <v>343</v>
+        <v>310</v>
       </c>
       <c r="O43" t="s">
-        <v>344</v>
+        <v>311</v>
+      </c>
+      <c r="P43" t="s">
+        <v>407</v>
       </c>
       <c r="Q43">
-        <v>38.664935999999997</v>
+        <v>34.574328000000001</v>
       </c>
       <c r="R43">
-        <v>-79.430160999999998</v>
-      </c>
-    </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
+        <v>-86.220834999999994</v>
+      </c>
+      <c r="W43" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="X43" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>183</v>
+        <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>184</v>
+        <v>206</v>
       </c>
       <c r="C44" t="s">
-        <v>183</v>
+        <v>47</v>
       </c>
       <c r="D44" s="5">
-        <v>6011472</v>
+        <v>3545533</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>185</v>
+        <v>207</v>
       </c>
       <c r="F44" t="s">
         <v>51</v>
       </c>
       <c r="G44" t="s">
-        <v>186</v>
+        <v>208</v>
       </c>
       <c r="H44">
-        <v>2010</v>
-      </c>
-      <c r="I44" s="1">
-        <v>40248</v>
+        <v>2016</v>
+      </c>
+      <c r="I44">
+        <v>2016</v>
       </c>
       <c r="J44" t="s">
-        <v>130</v>
+        <v>18</v>
       </c>
       <c r="K44" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="L44" t="s">
         <v>20</v>
       </c>
       <c r="M44" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="N44" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="O44" t="s">
-        <v>345</v>
+        <v>313</v>
+      </c>
+      <c r="P44" t="s">
+        <v>406</v>
       </c>
       <c r="Q44">
-        <v>48.174337000000001</v>
+        <v>47.550894599999999</v>
       </c>
       <c r="R44">
-        <v>-80.100126000000003</v>
+        <v>-121.53941880000001</v>
+      </c>
+      <c r="W44" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="X44" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>186</v>
+        <v>209</v>
       </c>
       <c r="B45" t="s">
-        <v>187</v>
+        <v>210</v>
       </c>
       <c r="C45" t="s">
-        <v>186</v>
+        <v>209</v>
       </c>
       <c r="D45" s="5">
-        <v>6011473</v>
+        <v>6011465</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="F45" t="s">
         <v>51</v>
       </c>
       <c r="G45" t="s">
-        <v>189</v>
+        <v>212</v>
       </c>
       <c r="H45">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="I45" s="1">
-        <v>40242</v>
+        <v>39901</v>
       </c>
       <c r="J45" t="s">
         <v>130</v>
@@ -9715,55 +9597,58 @@
       <c r="K45" t="s">
         <v>43</v>
       </c>
-      <c r="L45" t="s">
-        <v>20</v>
+      <c r="L45" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="M45" t="s">
-        <v>298</v>
+        <v>335</v>
       </c>
       <c r="N45" t="s">
-        <v>354</v>
+        <v>337</v>
       </c>
       <c r="O45" t="s">
-        <v>366</v>
+        <v>305</v>
       </c>
       <c r="Q45">
-        <v>36.555458999999999</v>
+        <v>47.145499999999998</v>
       </c>
       <c r="R45">
-        <v>-87.304068999999998</v>
+        <v>17.622399999999999</v>
+      </c>
+      <c r="X45" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="B46" t="s">
-        <v>190</v>
+        <v>213</v>
       </c>
       <c r="C46" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="D46" s="5">
-        <v>6011474</v>
+        <v>6011478</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>191</v>
+        <v>214</v>
       </c>
       <c r="F46" t="s">
         <v>51</v>
       </c>
       <c r="G46" t="s">
-        <v>192</v>
+        <v>215</v>
       </c>
       <c r="H46">
         <v>2008</v>
       </c>
       <c r="I46" s="1">
-        <v>39525</v>
+        <v>39539</v>
       </c>
       <c r="J46" t="s">
-        <v>193</v>
+        <v>130</v>
       </c>
       <c r="K46" t="s">
         <v>43</v>
@@ -9775,45 +9660,45 @@
         <v>298</v>
       </c>
       <c r="N46" t="s">
-        <v>304</v>
+        <v>349</v>
       </c>
       <c r="O46" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="Q46">
-        <v>42.871989999999997</v>
+        <v>41.745700999999997</v>
       </c>
       <c r="R46">
-        <v>-73.226607000000001</v>
+        <v>-73.158473999999998</v>
       </c>
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="B47" t="s">
-        <v>194</v>
+        <v>216</v>
       </c>
       <c r="C47" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="D47" s="5">
-        <v>6011475</v>
+        <v>6011479</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>195</v>
+        <v>217</v>
       </c>
       <c r="F47" t="s">
         <v>51</v>
       </c>
       <c r="G47" t="s">
-        <v>196</v>
+        <v>218</v>
       </c>
       <c r="H47">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="I47" s="1">
-        <v>39840</v>
+        <v>40217</v>
       </c>
       <c r="J47" t="s">
         <v>130</v>
@@ -9828,45 +9713,45 @@
         <v>298</v>
       </c>
       <c r="N47" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
       <c r="O47" t="s">
-        <v>350</v>
+        <v>365</v>
       </c>
       <c r="Q47">
-        <v>41.745700999999997</v>
+        <v>36.509321</v>
       </c>
       <c r="R47">
-        <v>-73.158473999999998</v>
+        <v>-82.328933000000006</v>
       </c>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="B48" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="C48" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="D48" s="5">
-        <v>6011476</v>
+        <v>6011480</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>198</v>
+        <v>220</v>
       </c>
       <c r="F48" t="s">
         <v>51</v>
       </c>
       <c r="G48" t="s">
-        <v>199</v>
+        <v>129</v>
       </c>
       <c r="H48">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="I48" s="1">
-        <v>39875</v>
+        <v>40242</v>
       </c>
       <c r="J48" t="s">
         <v>130</v>
@@ -9881,48 +9766,51 @@
         <v>298</v>
       </c>
       <c r="N48" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="O48" t="s">
-        <v>352</v>
+        <v>367</v>
       </c>
       <c r="Q48">
-        <v>37.322156999999997</v>
+        <v>39.69717</v>
       </c>
       <c r="R48">
-        <v>-80.756189000000006</v>
+        <v>-78.820670000000007</v>
+      </c>
+      <c r="X48" s="9" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>199</v>
+        <v>212</v>
       </c>
       <c r="B49" t="s">
-        <v>200</v>
+        <v>221</v>
       </c>
       <c r="C49" t="s">
-        <v>199</v>
+        <v>212</v>
       </c>
       <c r="D49" s="5">
-        <v>6011477</v>
+        <v>6011481</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>201</v>
+        <v>222</v>
       </c>
       <c r="F49" t="s">
         <v>51</v>
       </c>
       <c r="G49" t="s">
-        <v>202</v>
+        <v>223</v>
       </c>
       <c r="H49">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="I49" s="1">
-        <v>39528</v>
+        <v>39882</v>
       </c>
       <c r="J49" t="s">
-        <v>130</v>
+        <v>193</v>
       </c>
       <c r="K49" t="s">
         <v>43</v>
@@ -9934,51 +9822,51 @@
         <v>298</v>
       </c>
       <c r="N49" t="s">
-        <v>348</v>
+        <v>299</v>
       </c>
       <c r="O49" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="Q49">
-        <v>42.592351000000001</v>
+        <v>41.949971359391597</v>
       </c>
       <c r="R49">
-        <v>-73.226241999999999</v>
-      </c>
-    </row>
-    <row r="50" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+        <v>-74.288489118822994</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>41</v>
+        <v>134</v>
       </c>
       <c r="B50" t="s">
-        <v>203</v>
+        <v>224</v>
       </c>
       <c r="C50" t="s">
-        <v>41</v>
+        <v>134</v>
       </c>
       <c r="D50" s="5">
-        <v>3545532</v>
+        <v>6011482</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>204</v>
+        <v>225</v>
       </c>
       <c r="F50" t="s">
         <v>51</v>
       </c>
       <c r="G50" t="s">
-        <v>205</v>
+        <v>226</v>
       </c>
       <c r="H50">
-        <v>2015</v>
-      </c>
-      <c r="I50">
-        <v>2015</v>
+        <v>2010</v>
+      </c>
+      <c r="I50" s="1">
+        <v>40205</v>
       </c>
       <c r="J50" t="s">
-        <v>18</v>
+        <v>130</v>
       </c>
       <c r="K50" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="L50" t="s">
         <v>20</v>
@@ -9987,116 +9875,98 @@
         <v>298</v>
       </c>
       <c r="N50" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="O50" t="s">
-        <v>311</v>
-      </c>
-      <c r="P50" t="s">
-        <v>407</v>
+        <v>364</v>
       </c>
       <c r="Q50">
-        <v>34.574328000000001</v>
+        <v>43.451169999999998</v>
       </c>
       <c r="R50">
-        <v>-86.220834999999994</v>
-      </c>
-      <c r="W50" s="6" t="s">
-        <v>408</v>
-      </c>
-      <c r="X50" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="51" spans="1:24" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>-72.942554999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>47</v>
+        <v>138</v>
       </c>
       <c r="B51" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="C51" t="s">
-        <v>47</v>
+        <v>138</v>
       </c>
       <c r="D51" s="5">
-        <v>3545533</v>
+        <v>6011483</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>207</v>
+        <v>228</v>
       </c>
       <c r="F51" t="s">
         <v>51</v>
       </c>
       <c r="G51" t="s">
-        <v>208</v>
+        <v>229</v>
       </c>
       <c r="H51">
-        <v>2016</v>
-      </c>
-      <c r="I51">
-        <v>2016</v>
+        <v>2010</v>
+      </c>
+      <c r="I51" s="1">
+        <v>40252</v>
       </c>
       <c r="J51" t="s">
-        <v>18</v>
+        <v>130</v>
       </c>
       <c r="K51" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="L51" t="s">
         <v>20</v>
       </c>
       <c r="M51" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="N51" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="O51" t="s">
-        <v>313</v>
-      </c>
-      <c r="P51" t="s">
-        <v>406</v>
+        <v>305</v>
       </c>
       <c r="Q51">
-        <v>47.550894599999999</v>
+        <v>48.174337000000001</v>
       </c>
       <c r="R51">
-        <v>-121.53941880000001</v>
-      </c>
-      <c r="W51" s="6" t="s">
-        <v>408</v>
-      </c>
-      <c r="X51" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="52" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+        <v>-80.100126000000003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>209</v>
+        <v>142</v>
       </c>
       <c r="B52" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="C52" t="s">
-        <v>209</v>
+        <v>142</v>
       </c>
       <c r="D52" s="5">
-        <v>6011465</v>
+        <v>6011484</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
       <c r="F52" t="s">
-        <v>51</v>
+        <v>232</v>
       </c>
       <c r="G52" t="s">
-        <v>212</v>
+        <v>233</v>
       </c>
       <c r="H52">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="I52" s="1">
-        <v>39901</v>
+        <v>40275</v>
       </c>
       <c r="J52" t="s">
         <v>130</v>
@@ -10104,161 +9974,158 @@
       <c r="K52" t="s">
         <v>43</v>
       </c>
-      <c r="L52" s="10" t="s">
-        <v>25</v>
+      <c r="L52" t="s">
+        <v>20</v>
       </c>
       <c r="M52" t="s">
-        <v>335</v>
+        <v>298</v>
       </c>
       <c r="N52" t="s">
-        <v>337</v>
+        <v>354</v>
       </c>
       <c r="O52" t="s">
-        <v>305</v>
+        <v>368</v>
       </c>
       <c r="Q52">
-        <v>47.145499999999998</v>
+        <v>36.465316000000001</v>
       </c>
       <c r="R52">
-        <v>17.622399999999999</v>
-      </c>
-      <c r="X52" t="s">
-        <v>26</v>
+        <v>-84.971273999999994</v>
       </c>
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>202</v>
+        <v>150</v>
       </c>
       <c r="B53" t="s">
-        <v>213</v>
+        <v>234</v>
       </c>
       <c r="C53" t="s">
-        <v>202</v>
+        <v>150</v>
       </c>
       <c r="D53" s="5">
-        <v>6011478</v>
+        <v>6011486</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>214</v>
+        <v>235</v>
       </c>
       <c r="F53" t="s">
-        <v>51</v>
+        <v>232</v>
       </c>
       <c r="G53" t="s">
-        <v>215</v>
+        <v>233</v>
       </c>
       <c r="H53">
-        <v>2008</v>
-      </c>
-      <c r="I53" s="1">
-        <v>39539</v>
+        <v>2016</v>
+      </c>
+      <c r="I53">
+        <v>2016</v>
       </c>
       <c r="J53" t="s">
-        <v>130</v>
+        <v>42</v>
       </c>
       <c r="K53" t="s">
         <v>43</v>
       </c>
-      <c r="L53" t="s">
-        <v>20</v>
+      <c r="L53" s="10" t="s">
+        <v>236</v>
       </c>
       <c r="M53" t="s">
-        <v>298</v>
+        <v>237</v>
       </c>
       <c r="N53" t="s">
-        <v>349</v>
+        <v>305</v>
       </c>
       <c r="O53" t="s">
-        <v>350</v>
+        <v>237</v>
       </c>
       <c r="Q53">
-        <v>41.745700999999997</v>
+        <v>46.823079999999997</v>
       </c>
       <c r="R53">
-        <v>-73.158473999999998</v>
+        <v>102.503703</v>
       </c>
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>205</v>
+        <v>153</v>
       </c>
       <c r="B54" t="s">
-        <v>216</v>
+        <v>238</v>
       </c>
       <c r="C54" t="s">
-        <v>205</v>
+        <v>153</v>
       </c>
       <c r="D54" s="5">
-        <v>6011479</v>
+        <v>6011487</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>217</v>
+        <v>239</v>
       </c>
       <c r="F54" t="s">
-        <v>51</v>
+        <v>232</v>
       </c>
       <c r="G54" t="s">
-        <v>218</v>
+        <v>240</v>
       </c>
       <c r="H54">
-        <v>2010</v>
-      </c>
-      <c r="I54" s="1">
-        <v>40217</v>
+        <v>2016</v>
+      </c>
+      <c r="I54">
+        <v>2016</v>
       </c>
       <c r="J54" t="s">
-        <v>130</v>
+        <v>42</v>
       </c>
       <c r="K54" t="s">
         <v>43</v>
       </c>
-      <c r="L54" t="s">
-        <v>20</v>
+      <c r="L54" s="10" t="s">
+        <v>236</v>
       </c>
       <c r="M54" t="s">
-        <v>298</v>
+        <v>237</v>
       </c>
       <c r="N54" t="s">
-        <v>354</v>
+        <v>305</v>
       </c>
       <c r="O54" t="s">
-        <v>365</v>
+        <v>237</v>
       </c>
       <c r="Q54">
-        <v>36.509321</v>
+        <v>46.823079999999997</v>
       </c>
       <c r="R54">
-        <v>-82.328933000000006</v>
+        <v>102.503703</v>
       </c>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>208</v>
+        <v>157</v>
       </c>
       <c r="B55" t="s">
-        <v>219</v>
+        <v>241</v>
       </c>
       <c r="C55" t="s">
-        <v>208</v>
+        <v>157</v>
       </c>
       <c r="D55" s="5">
-        <v>6011480</v>
+        <v>6011488</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>220</v>
+        <v>242</v>
       </c>
       <c r="F55" t="s">
-        <v>51</v>
+        <v>232</v>
       </c>
       <c r="G55" t="s">
-        <v>129</v>
+        <v>243</v>
       </c>
       <c r="H55">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="I55" s="1">
-        <v>40242</v>
+        <v>41011</v>
       </c>
       <c r="J55" t="s">
         <v>130</v>
@@ -10270,54 +10137,51 @@
         <v>20</v>
       </c>
       <c r="M55" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="N55" t="s">
-        <v>355</v>
+        <v>292</v>
       </c>
       <c r="O55" t="s">
-        <v>367</v>
+        <v>297</v>
       </c>
       <c r="Q55">
-        <v>39.69717</v>
+        <v>45.93694</v>
       </c>
       <c r="R55">
-        <v>-78.820670000000007</v>
-      </c>
-      <c r="X55" s="9" t="s">
-        <v>417</v>
+        <v>-64.476939999999999</v>
       </c>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>212</v>
+        <v>161</v>
       </c>
       <c r="B56" t="s">
-        <v>221</v>
+        <v>244</v>
       </c>
       <c r="C56" t="s">
-        <v>212</v>
+        <v>161</v>
       </c>
       <c r="D56" s="5">
-        <v>6011481</v>
+        <v>6011489</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>222</v>
+        <v>245</v>
       </c>
       <c r="F56" t="s">
-        <v>51</v>
+        <v>232</v>
       </c>
       <c r="G56" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="H56">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="I56" s="1">
-        <v>39882</v>
+        <v>40987</v>
       </c>
       <c r="J56" t="s">
-        <v>193</v>
+        <v>117</v>
       </c>
       <c r="K56" t="s">
         <v>43</v>
@@ -10329,45 +10193,45 @@
         <v>298</v>
       </c>
       <c r="N56" t="s">
-        <v>299</v>
+        <v>359</v>
       </c>
       <c r="O56" t="s">
-        <v>353</v>
+        <v>374</v>
       </c>
       <c r="Q56">
-        <v>41.949971359391597</v>
+        <v>39.048609999999996</v>
       </c>
       <c r="R56">
-        <v>-74.288489118822994</v>
+        <v>-90.88167</v>
       </c>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>134</v>
+        <v>246</v>
       </c>
       <c r="B57" t="s">
-        <v>224</v>
+        <v>247</v>
       </c>
       <c r="C57" t="s">
-        <v>134</v>
+        <v>246</v>
       </c>
       <c r="D57" s="5">
-        <v>6011482</v>
+        <v>6011490</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>225</v>
+        <v>248</v>
       </c>
       <c r="F57" t="s">
-        <v>51</v>
+        <v>232</v>
       </c>
       <c r="G57" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="H57">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="I57" s="1">
-        <v>40205</v>
+        <v>40590</v>
       </c>
       <c r="J57" t="s">
         <v>130</v>
@@ -10382,45 +10246,45 @@
         <v>298</v>
       </c>
       <c r="N57" t="s">
-        <v>304</v>
+        <v>351</v>
       </c>
       <c r="O57" t="s">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="Q57">
-        <v>43.451169999999998</v>
+        <v>36.968234063873403</v>
       </c>
       <c r="R57">
-        <v>-72.942554999999999</v>
+        <v>-82.639469435652799</v>
       </c>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="B58" t="s">
-        <v>227</v>
+        <v>249</v>
       </c>
       <c r="C58" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="D58" s="5">
-        <v>6011483</v>
+        <v>6011491</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>228</v>
+        <v>250</v>
       </c>
       <c r="F58" t="s">
-        <v>51</v>
+        <v>232</v>
       </c>
       <c r="G58" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
       <c r="H58">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="I58" s="1">
-        <v>40252</v>
+        <v>40583</v>
       </c>
       <c r="J58" t="s">
         <v>130</v>
@@ -10432,48 +10296,48 @@
         <v>20</v>
       </c>
       <c r="M58" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="N58" t="s">
-        <v>319</v>
+        <v>354</v>
       </c>
       <c r="O58" t="s">
-        <v>305</v>
+        <v>366</v>
       </c>
       <c r="Q58">
-        <v>48.174337000000001</v>
+        <v>36.555458999999999</v>
       </c>
       <c r="R58">
-        <v>-80.100126000000003</v>
+        <v>-87.304068999999998</v>
       </c>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>142</v>
+        <v>251</v>
       </c>
       <c r="B59" t="s">
-        <v>230</v>
+        <v>252</v>
       </c>
       <c r="C59" t="s">
-        <v>142</v>
+        <v>251</v>
       </c>
       <c r="D59" s="5">
-        <v>6011484</v>
+        <v>6011492</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>231</v>
+        <v>253</v>
       </c>
       <c r="F59" t="s">
         <v>232</v>
       </c>
       <c r="G59" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
       <c r="H59">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="I59" s="1">
-        <v>40275</v>
+        <v>40572</v>
       </c>
       <c r="J59" t="s">
         <v>130</v>
@@ -10488,154 +10352,154 @@
         <v>298</v>
       </c>
       <c r="N59" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="O59" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="Q59">
-        <v>36.465316000000001</v>
+        <v>38.229909999999997</v>
       </c>
       <c r="R59">
-        <v>-84.971273999999994</v>
-      </c>
-    </row>
-    <row r="60" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+        <v>-86.294910000000002</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>150</v>
+        <v>254</v>
       </c>
       <c r="B60" t="s">
-        <v>234</v>
+        <v>255</v>
       </c>
       <c r="C60" t="s">
-        <v>150</v>
+        <v>254</v>
       </c>
       <c r="D60" s="5">
-        <v>6011486</v>
+        <v>6011493</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>235</v>
+        <v>256</v>
       </c>
       <c r="F60" t="s">
         <v>232</v>
       </c>
       <c r="G60" t="s">
-        <v>233</v>
+        <v>257</v>
       </c>
       <c r="H60">
-        <v>2016</v>
-      </c>
-      <c r="I60">
-        <v>2016</v>
+        <v>2011</v>
+      </c>
+      <c r="I60" s="1">
+        <v>40566</v>
       </c>
       <c r="J60" t="s">
-        <v>42</v>
+        <v>193</v>
       </c>
       <c r="K60" t="s">
         <v>43</v>
       </c>
-      <c r="L60" s="10" t="s">
-        <v>236</v>
+      <c r="L60" t="s">
+        <v>20</v>
       </c>
       <c r="M60" t="s">
-        <v>237</v>
+        <v>298</v>
       </c>
       <c r="N60" t="s">
-        <v>305</v>
+        <v>356</v>
       </c>
       <c r="O60" t="s">
-        <v>237</v>
+        <v>369</v>
       </c>
       <c r="Q60">
-        <v>46.823079999999997</v>
+        <v>38.702026438267701</v>
       </c>
       <c r="R60">
-        <v>102.503703</v>
-      </c>
-    </row>
-    <row r="61" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+        <v>-86.233603821942907</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>153</v>
+        <v>258</v>
       </c>
       <c r="B61" t="s">
-        <v>238</v>
+        <v>259</v>
       </c>
       <c r="C61" t="s">
-        <v>153</v>
+        <v>258</v>
       </c>
       <c r="D61" s="5">
-        <v>6011487</v>
+        <v>6011494</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>239</v>
+        <v>260</v>
       </c>
       <c r="F61" t="s">
         <v>232</v>
       </c>
       <c r="G61" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
       <c r="H61">
-        <v>2016</v>
-      </c>
-      <c r="I61">
-        <v>2016</v>
+        <v>2012</v>
+      </c>
+      <c r="I61" s="1">
+        <v>40969</v>
       </c>
       <c r="J61" t="s">
-        <v>42</v>
+        <v>117</v>
       </c>
       <c r="K61" t="s">
         <v>43</v>
       </c>
-      <c r="L61" s="10" t="s">
-        <v>236</v>
+      <c r="L61" t="s">
+        <v>20</v>
       </c>
       <c r="M61" t="s">
-        <v>237</v>
+        <v>298</v>
       </c>
       <c r="N61" t="s">
-        <v>305</v>
+        <v>358</v>
       </c>
       <c r="O61" t="s">
-        <v>237</v>
+        <v>373</v>
       </c>
       <c r="Q61">
-        <v>46.823079999999997</v>
+        <v>39.838700000000003</v>
       </c>
       <c r="R61">
-        <v>102.503703</v>
+        <v>-75.563800000000001</v>
       </c>
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>157</v>
+        <v>215</v>
       </c>
       <c r="B62" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
       <c r="C62" t="s">
-        <v>157</v>
+        <v>215</v>
       </c>
       <c r="D62" s="5">
-        <v>6011488</v>
+        <v>6011495</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
       <c r="F62" t="s">
-        <v>232</v>
+        <v>51</v>
       </c>
       <c r="G62" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="H62">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="I62" s="1">
-        <v>41011</v>
+        <v>40889</v>
       </c>
       <c r="J62" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="K62" t="s">
         <v>43</v>
@@ -10644,48 +10508,51 @@
         <v>20</v>
       </c>
       <c r="M62" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="N62" t="s">
-        <v>292</v>
+        <v>357</v>
       </c>
       <c r="O62" t="s">
-        <v>297</v>
+        <v>372</v>
       </c>
       <c r="Q62">
-        <v>45.93694</v>
+        <v>44.349651999999999</v>
       </c>
       <c r="R62">
-        <v>-64.476939999999999</v>
+        <v>-68.211070000000007</v>
+      </c>
+      <c r="X62" s="9" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>161</v>
+        <v>264</v>
       </c>
       <c r="B63" t="s">
-        <v>244</v>
+        <v>265</v>
       </c>
       <c r="C63" t="s">
-        <v>161</v>
+        <v>264</v>
       </c>
       <c r="D63" s="5">
-        <v>6011489</v>
+        <v>6011496</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>245</v>
+        <v>266</v>
       </c>
       <c r="F63" t="s">
-        <v>232</v>
+        <v>51</v>
       </c>
       <c r="G63" t="s">
-        <v>233</v>
+        <v>267</v>
       </c>
       <c r="H63">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="I63" s="1">
-        <v>40987</v>
+        <v>40577</v>
       </c>
       <c r="J63" t="s">
         <v>117</v>
@@ -10693,108 +10560,114 @@
       <c r="K63" t="s">
         <v>43</v>
       </c>
-      <c r="L63" t="s">
-        <v>20</v>
+      <c r="L63" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="M63" t="s">
-        <v>298</v>
+        <v>268</v>
       </c>
       <c r="N63" t="s">
-        <v>359</v>
+        <v>305</v>
       </c>
       <c r="O63" t="s">
-        <v>374</v>
+        <v>305</v>
       </c>
       <c r="Q63">
-        <v>39.048609999999996</v>
+        <v>50.45</v>
       </c>
       <c r="R63">
-        <v>-90.88167</v>
+        <v>30.5</v>
+      </c>
+      <c r="X63" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="64" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>246</v>
+        <v>269</v>
       </c>
       <c r="B64" t="s">
-        <v>247</v>
+        <v>270</v>
       </c>
       <c r="C64" t="s">
-        <v>246</v>
+        <v>269</v>
       </c>
       <c r="D64" s="5">
-        <v>6011490</v>
+        <v>6011497</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>248</v>
+        <v>271</v>
       </c>
       <c r="F64" t="s">
-        <v>232</v>
+        <v>51</v>
       </c>
       <c r="G64" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="H64">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="I64" s="1">
-        <v>40590</v>
+        <v>39884</v>
       </c>
       <c r="J64" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="K64" t="s">
         <v>43</v>
       </c>
-      <c r="L64" t="s">
-        <v>20</v>
+      <c r="L64" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="M64" t="s">
-        <v>298</v>
+        <v>346</v>
       </c>
       <c r="N64" t="s">
-        <v>351</v>
+        <v>363</v>
       </c>
       <c r="O64" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="Q64">
-        <v>36.968234063873403</v>
+        <v>45.1</v>
       </c>
       <c r="R64">
-        <v>-82.639469435652799</v>
-      </c>
-    </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.2">
+        <v>0.7</v>
+      </c>
+      <c r="X64" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>164</v>
+        <v>273</v>
       </c>
       <c r="B65" t="s">
-        <v>249</v>
+        <v>274</v>
       </c>
       <c r="C65" t="s">
-        <v>164</v>
+        <v>273</v>
       </c>
       <c r="D65" s="5">
-        <v>6011491</v>
+        <v>11812088</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>250</v>
+        <v>275</v>
       </c>
       <c r="F65" t="s">
-        <v>232</v>
+        <v>51</v>
       </c>
       <c r="G65" t="s">
-        <v>240</v>
+        <v>276</v>
       </c>
       <c r="H65">
-        <v>2011</v>
-      </c>
-      <c r="I65" s="1">
-        <v>40583</v>
+        <v>2014</v>
+      </c>
+      <c r="I65">
+        <v>2014</v>
       </c>
       <c r="J65" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="K65" t="s">
         <v>43</v>
@@ -10803,51 +10676,51 @@
         <v>20</v>
       </c>
       <c r="M65" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="N65" t="s">
-        <v>354</v>
+        <v>319</v>
       </c>
       <c r="O65" t="s">
-        <v>366</v>
+        <v>334</v>
       </c>
       <c r="Q65">
-        <v>36.555458999999999</v>
+        <v>43.468915000000003</v>
       </c>
       <c r="R65">
-        <v>-87.304068999999998</v>
-      </c>
-    </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.2">
+        <v>-79.911533000000006</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>251</v>
+        <v>277</v>
       </c>
       <c r="B66" t="s">
-        <v>252</v>
+        <v>278</v>
       </c>
       <c r="C66" t="s">
-        <v>251</v>
+        <v>277</v>
       </c>
       <c r="D66" s="5">
-        <v>6011492</v>
+        <v>11812089</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>253</v>
+        <v>279</v>
       </c>
       <c r="F66" t="s">
-        <v>232</v>
+        <v>51</v>
       </c>
       <c r="G66" t="s">
-        <v>243</v>
+        <v>280</v>
       </c>
       <c r="H66">
-        <v>2011</v>
-      </c>
-      <c r="I66" s="1">
-        <v>40572</v>
+        <v>2013</v>
+      </c>
+      <c r="I66">
+        <v>2013</v>
       </c>
       <c r="J66" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="K66" t="s">
         <v>43</v>
@@ -10856,51 +10729,51 @@
         <v>20</v>
       </c>
       <c r="M66" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="N66" t="s">
-        <v>356</v>
+        <v>322</v>
       </c>
       <c r="O66" t="s">
-        <v>370</v>
+        <v>333</v>
       </c>
       <c r="Q66">
-        <v>38.229909999999997</v>
+        <v>44.992969000000002</v>
       </c>
       <c r="R66">
-        <v>-86.294910000000002</v>
-      </c>
-    </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.2">
+        <v>-64.167955000000006</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>254</v>
+        <v>281</v>
       </c>
       <c r="B67" t="s">
-        <v>255</v>
+        <v>282</v>
       </c>
       <c r="C67" t="s">
-        <v>254</v>
+        <v>281</v>
       </c>
       <c r="D67" s="5">
-        <v>6011493</v>
+        <v>11812090</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
       <c r="F67" t="s">
-        <v>232</v>
+        <v>16</v>
       </c>
       <c r="G67" t="s">
-        <v>257</v>
+        <v>284</v>
       </c>
       <c r="H67">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="I67" s="1">
-        <v>40566</v>
+        <v>40967</v>
       </c>
       <c r="J67" t="s">
-        <v>193</v>
+        <v>117</v>
       </c>
       <c r="K67" t="s">
         <v>43</v>
@@ -10909,48 +10782,48 @@
         <v>20</v>
       </c>
       <c r="M67" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="N67" t="s">
-        <v>356</v>
+        <v>292</v>
       </c>
       <c r="O67" t="s">
-        <v>369</v>
+        <v>332</v>
       </c>
       <c r="Q67">
-        <v>38.702026438267701</v>
+        <v>45.300289999999997</v>
       </c>
       <c r="R67">
-        <v>-86.233603821942907</v>
-      </c>
-    </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.2">
+        <v>-66.050550000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>258</v>
+        <v>285</v>
       </c>
       <c r="B68" t="s">
-        <v>259</v>
+        <v>286</v>
       </c>
       <c r="C68" t="s">
-        <v>258</v>
+        <v>285</v>
       </c>
       <c r="D68" s="5">
-        <v>6011494</v>
+        <v>11812091</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>260</v>
+        <v>287</v>
       </c>
       <c r="F68" t="s">
-        <v>232</v>
+        <v>51</v>
       </c>
       <c r="G68" t="s">
-        <v>257</v>
+        <v>288</v>
       </c>
       <c r="H68">
         <v>2012</v>
       </c>
-      <c r="I68" s="1">
-        <v>40969</v>
+      <c r="I68">
+        <v>2012</v>
       </c>
       <c r="J68" t="s">
         <v>117</v>
@@ -10962,419 +10835,38 @@
         <v>20</v>
       </c>
       <c r="M68" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="N68" t="s">
-        <v>358</v>
+        <v>292</v>
       </c>
       <c r="O68" t="s">
-        <v>373</v>
+        <v>297</v>
       </c>
       <c r="Q68">
-        <v>39.838700000000003</v>
+        <v>45.93694</v>
       </c>
       <c r="R68">
-        <v>-75.563800000000001</v>
-      </c>
-    </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>215</v>
-      </c>
-      <c r="B69" t="s">
-        <v>261</v>
-      </c>
-      <c r="C69" t="s">
-        <v>215</v>
-      </c>
-      <c r="D69" s="5">
-        <v>6011495</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="F69" t="s">
-        <v>51</v>
-      </c>
-      <c r="G69" t="s">
-        <v>263</v>
-      </c>
-      <c r="H69">
-        <v>2011</v>
-      </c>
-      <c r="I69" s="1">
-        <v>40889</v>
-      </c>
-      <c r="J69" t="s">
-        <v>117</v>
-      </c>
-      <c r="K69" t="s">
-        <v>43</v>
-      </c>
-      <c r="L69" t="s">
-        <v>20</v>
-      </c>
-      <c r="M69" t="s">
-        <v>298</v>
-      </c>
-      <c r="N69" t="s">
-        <v>357</v>
-      </c>
-      <c r="O69" t="s">
-        <v>372</v>
-      </c>
-      <c r="Q69">
-        <v>44.349651999999999</v>
-      </c>
-      <c r="R69">
-        <v>-68.211070000000007</v>
-      </c>
-      <c r="X69" s="9" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="70" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>264</v>
-      </c>
-      <c r="B70" t="s">
-        <v>265</v>
-      </c>
-      <c r="C70" t="s">
-        <v>264</v>
-      </c>
-      <c r="D70" s="5">
-        <v>6011496</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="F70" t="s">
-        <v>51</v>
-      </c>
-      <c r="G70" t="s">
-        <v>267</v>
-      </c>
-      <c r="H70">
-        <v>2011</v>
-      </c>
-      <c r="I70" s="1">
-        <v>40577</v>
-      </c>
-      <c r="J70" t="s">
-        <v>117</v>
-      </c>
-      <c r="K70" t="s">
-        <v>43</v>
-      </c>
-      <c r="L70" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="M70" t="s">
-        <v>268</v>
-      </c>
-      <c r="N70" t="s">
-        <v>305</v>
-      </c>
-      <c r="O70" t="s">
-        <v>305</v>
-      </c>
-      <c r="Q70">
-        <v>50.45</v>
-      </c>
-      <c r="R70">
-        <v>30.5</v>
-      </c>
-      <c r="X70" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="71" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>269</v>
-      </c>
-      <c r="B71" t="s">
-        <v>270</v>
-      </c>
-      <c r="C71" t="s">
-        <v>269</v>
-      </c>
-      <c r="D71" s="5">
-        <v>6011497</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="F71" t="s">
-        <v>51</v>
-      </c>
-      <c r="G71" t="s">
-        <v>272</v>
-      </c>
-      <c r="H71">
-        <v>2009</v>
-      </c>
-      <c r="I71" s="1">
-        <v>39884</v>
-      </c>
-      <c r="J71" t="s">
-        <v>117</v>
-      </c>
-      <c r="K71" t="s">
-        <v>43</v>
-      </c>
-      <c r="L71" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="M71" t="s">
-        <v>346</v>
-      </c>
-      <c r="N71" t="s">
-        <v>363</v>
-      </c>
-      <c r="O71" t="s">
-        <v>362</v>
-      </c>
-      <c r="Q71">
-        <v>45.1</v>
-      </c>
-      <c r="R71">
-        <v>0.7</v>
-      </c>
-      <c r="X71" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>273</v>
-      </c>
-      <c r="B72" t="s">
-        <v>274</v>
-      </c>
-      <c r="C72" t="s">
-        <v>273</v>
-      </c>
-      <c r="D72" s="5">
-        <v>11812088</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="F72" t="s">
-        <v>51</v>
-      </c>
-      <c r="G72" t="s">
-        <v>276</v>
-      </c>
-      <c r="H72">
-        <v>2014</v>
-      </c>
-      <c r="I72">
-        <v>2014</v>
-      </c>
-      <c r="J72" t="s">
-        <v>117</v>
-      </c>
-      <c r="K72" t="s">
-        <v>43</v>
-      </c>
-      <c r="L72" t="s">
-        <v>20</v>
-      </c>
-      <c r="M72" t="s">
-        <v>291</v>
-      </c>
-      <c r="N72" t="s">
-        <v>319</v>
-      </c>
-      <c r="O72" t="s">
-        <v>334</v>
-      </c>
-      <c r="Q72">
-        <v>43.468915000000003</v>
-      </c>
-      <c r="R72">
-        <v>-79.911533000000006</v>
-      </c>
-    </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>277</v>
-      </c>
-      <c r="B73" t="s">
-        <v>278</v>
-      </c>
-      <c r="C73" t="s">
-        <v>277</v>
-      </c>
-      <c r="D73" s="5">
-        <v>11812089</v>
-      </c>
-      <c r="E73" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="F73" t="s">
-        <v>51</v>
-      </c>
-      <c r="G73" t="s">
-        <v>280</v>
-      </c>
-      <c r="H73">
-        <v>2013</v>
-      </c>
-      <c r="I73">
-        <v>2013</v>
-      </c>
-      <c r="J73" t="s">
-        <v>117</v>
-      </c>
-      <c r="K73" t="s">
-        <v>43</v>
-      </c>
-      <c r="L73" t="s">
-        <v>20</v>
-      </c>
-      <c r="M73" t="s">
-        <v>291</v>
-      </c>
-      <c r="N73" t="s">
-        <v>322</v>
-      </c>
-      <c r="O73" t="s">
-        <v>333</v>
-      </c>
-      <c r="Q73">
-        <v>44.992969000000002</v>
-      </c>
-      <c r="R73">
-        <v>-64.167955000000006</v>
-      </c>
-    </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>281</v>
-      </c>
-      <c r="B74" t="s">
-        <v>282</v>
-      </c>
-      <c r="C74" t="s">
-        <v>281</v>
-      </c>
-      <c r="D74" s="5">
-        <v>11812090</v>
-      </c>
-      <c r="E74" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="F74" t="s">
-        <v>16</v>
-      </c>
-      <c r="G74" t="s">
-        <v>284</v>
-      </c>
-      <c r="H74">
-        <v>2012</v>
-      </c>
-      <c r="I74" s="1">
-        <v>40967</v>
-      </c>
-      <c r="J74" t="s">
-        <v>117</v>
-      </c>
-      <c r="K74" t="s">
-        <v>43</v>
-      </c>
-      <c r="L74" t="s">
-        <v>20</v>
-      </c>
-      <c r="M74" t="s">
-        <v>291</v>
-      </c>
-      <c r="N74" t="s">
-        <v>292</v>
-      </c>
-      <c r="O74" t="s">
-        <v>332</v>
-      </c>
-      <c r="Q74">
-        <v>45.300289999999997</v>
-      </c>
-      <c r="R74">
-        <v>-66.050550000000001</v>
-      </c>
-    </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>285</v>
-      </c>
-      <c r="B75" t="s">
-        <v>286</v>
-      </c>
-      <c r="C75" t="s">
-        <v>285</v>
-      </c>
-      <c r="D75" s="5">
-        <v>11812091</v>
-      </c>
-      <c r="E75" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="F75" t="s">
-        <v>51</v>
-      </c>
-      <c r="G75" t="s">
-        <v>288</v>
-      </c>
-      <c r="H75">
-        <v>2012</v>
-      </c>
-      <c r="I75">
-        <v>2012</v>
-      </c>
-      <c r="J75" t="s">
-        <v>117</v>
-      </c>
-      <c r="K75" t="s">
-        <v>43</v>
-      </c>
-      <c r="L75" t="s">
-        <v>20</v>
-      </c>
-      <c r="M75" t="s">
-        <v>291</v>
-      </c>
-      <c r="N75" t="s">
-        <v>292</v>
-      </c>
-      <c r="O75" t="s">
-        <v>297</v>
-      </c>
-      <c r="Q75">
-        <v>45.93694</v>
-      </c>
-      <c r="R75">
         <v>-64.476939999999999</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="W35" r:id="rId1" xr:uid="{30B91538-5C57-1447-95BD-AC8369DA5F5E}"/>
-    <hyperlink ref="W3:W5" r:id="rId2" display="https://www.broadinstitute.org/fungal-genome-initiative/geomyces-destructans-genome-project" xr:uid="{D37B37A2-3EBA-CA4E-854A-E666F7D90D9E}"/>
-    <hyperlink ref="W27" r:id="rId3" xr:uid="{B7DF38F8-BAD1-9945-B8D1-11D515725C8F}"/>
-    <hyperlink ref="W7:W13" r:id="rId4" display="https://doi.org/10.1038/s41467-017-02441-z" xr:uid="{B0C247A6-7615-4045-96A3-37610293BF68}"/>
-    <hyperlink ref="W5" r:id="rId5" xr:uid="{A95CF209-4DFD-CD4F-9B3C-1402FCA6D700}"/>
-    <hyperlink ref="W29" r:id="rId6" xr:uid="{FFDE2E21-2A9D-524E-9E52-4427DFB020CF}"/>
-    <hyperlink ref="W2" r:id="rId7" xr:uid="{2EBFD348-FAF0-7940-9B79-BBFE6D4A8266}"/>
-    <hyperlink ref="W50" r:id="rId8" xr:uid="{6B8A706E-D16F-7E48-8871-C6BC14742A22}"/>
-    <hyperlink ref="W51" r:id="rId9" xr:uid="{D18D0BED-E12E-9E44-953C-AD261B4B1885}"/>
-    <hyperlink ref="X55" r:id="rId10" location="close --&gt; used to find  most clustered group of caves in the county" xr:uid="{FE171B62-9507-F44D-A4C8-93F2E8E19CF0}"/>
-    <hyperlink ref="X69" r:id="rId11" xr:uid="{6AF0CD04-00AA-6F4C-A67F-FD31C4C9A051}"/>
+    <hyperlink ref="W28" r:id="rId1" xr:uid="{3DA3BF50-C718-4042-AB38-8735C412C066}"/>
+    <hyperlink ref="W3:W5" r:id="rId2" display="https://www.broadinstitute.org/fungal-genome-initiative/geomyces-destructans-genome-project" xr:uid="{1AAC961A-6EDA-4148-9B4F-0CA1532C4848}"/>
+    <hyperlink ref="W27" r:id="rId3" xr:uid="{9413F2DF-9CF6-5A47-9263-53F94E6E38F0}"/>
+    <hyperlink ref="W7:W13" r:id="rId4" display="https://doi.org/10.1038/s41467-017-02441-z" xr:uid="{10FFF060-2B2E-064B-83CE-CE5C13A4C475}"/>
+    <hyperlink ref="W5" r:id="rId5" xr:uid="{AA3197C4-28D6-7F45-809F-3D3F6942E815}"/>
+    <hyperlink ref="W2" r:id="rId6" xr:uid="{BD924FBD-C0DE-C744-B59B-8D2DA9D331DE}"/>
+    <hyperlink ref="W43" r:id="rId7" xr:uid="{90F9021C-5B1B-6240-BAA5-2E9F79A0155A}"/>
+    <hyperlink ref="W44" r:id="rId8" xr:uid="{2594ECE7-B238-6940-A003-2BD99A0CB6A2}"/>
+    <hyperlink ref="X48" r:id="rId9" location="close --&gt; used to find  most clustered group of caves in the county" xr:uid="{92A2A68F-4C43-8149-AF16-4E3ECAC1437F}"/>
+    <hyperlink ref="X62" r:id="rId10" xr:uid="{C7F50DBF-DBBD-8F40-84B6-E18DD5C9F49C}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
-    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
@@ -15518,8 +15010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ACF0E31-960B-2445-8C48-EBC2D8B4142C}">
   <dimension ref="A1:Y51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -15557,7 +15049,7 @@
       <c r="F1" s="11" t="s">
         <v>395</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="31" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="11" t="s">
@@ -15569,10 +15061,10 @@
       <c r="J1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="K1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="L1" s="31" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="11" t="s">
@@ -17821,7 +17313,7 @@
       <c r="V35" s="13"/>
       <c r="W35" s="13"/>
       <c r="X35" s="26"/>
-      <c r="Y35" s="30" t="s">
+      <c r="Y35" s="9" t="s">
         <v>417</v>
       </c>
     </row>
@@ -18555,7 +18047,7 @@
       <c r="V47" s="13"/>
       <c r="W47" s="13"/>
       <c r="X47" s="26"/>
-      <c r="Y47" s="30" t="s">
+      <c r="Y47" s="9" t="s">
         <v>418</v>
       </c>
     </row>
@@ -18800,7 +18292,7 @@
       <c r="U51" s="14"/>
       <c r="V51" s="14"/>
       <c r="W51" s="14"/>
-      <c r="X51" s="31"/>
+      <c r="X51" s="30"/>
       <c r="Y51" s="14"/>
     </row>
   </sheetData>

</xml_diff>